<commit_message>
Updated Brewery Bar listings
Added Woodforde's Brewery to the listings and updated the webpage.
</commit_message>
<xml_diff>
--- a/listings/brewery-bars.xlsx
+++ b/listings/brewery-bars.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="157">
   <si>
     <t>Brewery</t>
   </si>
@@ -425,6 +425,63 @@
   </si>
   <si>
     <t>Mead beer</t>
+  </si>
+  <si>
+    <t>Woodforde's Brewery</t>
+  </si>
+  <si>
+    <t>Wherry (Amber Ale)</t>
+  </si>
+  <si>
+    <t>A Supreme Champion Beer of Britain! Mighty fresh and zesty, our award-winning, rich amber ale enjoys floods of flavours, as sweet malts clash with grapefruit hops and big floral aromas in a sensory strike. Set sail on an epic taste adventure.</t>
+  </si>
+  <si>
+    <t>Reedlighter (Pale Ale)</t>
+  </si>
+  <si>
+    <t>Light and refreshing, this beer has been crafted with a blend of our finest hops. Paired up with malt blends and splashes of fresh, citrus flavours, this lightly coloured hoppy delight is designed to entice.</t>
+  </si>
+  <si>
+    <t>Bure Gold (Golden Ale)</t>
+  </si>
+  <si>
+    <t>We’ve meticulously selected the pale and lightly-roasted malts to form a classic aromatic, golden ale with notes of passionfruit and orange. Sailing to the far reaches, we’ve found hops from America and Slovenia, combined with the best of British. Bring home the gold.</t>
+  </si>
+  <si>
+    <t>Nelson's Revenge (Bitter)</t>
+  </si>
+  <si>
+    <t>Revenge is best served bittersweet. Our wholehearted harmony of hops, fruits and barley pays homage to brave Admiral Nelson and his crew. Nelson’s is a Norfolk beer, and glory in the taste and aromas of citrus and Norfolk malts we’ve crammed in.</t>
+  </si>
+  <si>
+    <t>Norfolk Nog (Dark Ale)</t>
+  </si>
+  <si>
+    <t>A Supreme Champion Beer of Britain! Our deep, ruby-red ale graces the senses with comforting splashes of warm hints. Inside, you’ll find a rich, chocolatey taste, tucked away with liquorice and treacle. All enveloped in a velvety blanket, for a smooth, unmistakable texture and finish.</t>
+  </si>
+  <si>
+    <t>Once Bittern (Bitter)</t>
+  </si>
+  <si>
+    <t>The rich spice and citrus fruit aromas in this beer echo the majestic calls of the Norfolk Bittern. Fittingly copper-coloured, with hints of sweet malt and fruit, our dry-finished beer came home to roost in Norfolk and is here to stay.</t>
+  </si>
+  <si>
+    <t>Mardler's (Mild Ale)</t>
+  </si>
+  <si>
+    <t>A dark, mild ale taking its name from an ancient Norfolk dialect — ‘to chat’. With delicate sweet roasted malts, and a low hopping rate, share a conversation over this special session brew: a beer worth talking about.</t>
+  </si>
+  <si>
+    <t>Red Admiral (Red Rye Ale)</t>
+  </si>
+  <si>
+    <t>A rye beer to conquer the senses. This alluring, deep ruby ale fuses spicy fruit and lightly malted hops in a harmony of sweet and bitter tastes. When days are getting shorter, make more of your evenings with Red Admiral’s big combo of flavours for an even bigger brew.</t>
+  </si>
+  <si>
+    <t>Volt (Pale Ale)</t>
+  </si>
+  <si>
+    <t>A beer with some serious voltage. This IPA is crafted to spark your taste buds. The best American hops are all piled into this beer. Tropical, citrus, floral and pine can all be found in one of our most aromatic brews. Shock the system.</t>
   </si>
 </sst>
 </file>
@@ -475,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -499,6 +556,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -1428,2812 +1488,2911 @@
       </c>
     </row>
     <row r="65">
-      <c r="D65" s="8"/>
+      <c r="A65" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="66">
-      <c r="D66" s="8"/>
+      <c r="A66" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C66" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="67">
-      <c r="D67" s="8"/>
+      <c r="A67" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C67" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="68">
-      <c r="D68" s="8"/>
+      <c r="A68" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="69">
-      <c r="D69" s="8"/>
+      <c r="A69" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" s="3">
+        <v>4.6</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="70">
-      <c r="D70" s="8"/>
+      <c r="A70" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C70" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="71">
-      <c r="D71" s="8"/>
+      <c r="A71" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C71" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="72">
-      <c r="D72" s="8"/>
+      <c r="A72" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="73">
-      <c r="D73" s="8"/>
+      <c r="A73" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C73" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="74">
-      <c r="D74" s="8"/>
+      <c r="D74" s="9"/>
     </row>
     <row r="75">
-      <c r="D75" s="8"/>
+      <c r="D75" s="9"/>
     </row>
     <row r="76">
-      <c r="D76" s="8"/>
+      <c r="D76" s="9"/>
     </row>
     <row r="77">
-      <c r="D77" s="8"/>
+      <c r="D77" s="9"/>
     </row>
     <row r="78">
-      <c r="D78" s="8"/>
+      <c r="D78" s="9"/>
     </row>
     <row r="79">
-      <c r="D79" s="8"/>
+      <c r="D79" s="9"/>
     </row>
     <row r="80">
-      <c r="D80" s="8"/>
+      <c r="D80" s="9"/>
     </row>
     <row r="81">
-      <c r="D81" s="8"/>
+      <c r="D81" s="9"/>
     </row>
     <row r="82">
-      <c r="D82" s="8"/>
+      <c r="D82" s="9"/>
     </row>
     <row r="83">
-      <c r="D83" s="8"/>
+      <c r="D83" s="9"/>
     </row>
     <row r="84">
-      <c r="D84" s="8"/>
+      <c r="D84" s="9"/>
     </row>
     <row r="85">
-      <c r="D85" s="8"/>
+      <c r="D85" s="9"/>
     </row>
     <row r="86">
-      <c r="D86" s="8"/>
+      <c r="D86" s="9"/>
     </row>
     <row r="87">
-      <c r="D87" s="8"/>
+      <c r="D87" s="9"/>
     </row>
     <row r="88">
-      <c r="D88" s="8"/>
+      <c r="D88" s="9"/>
     </row>
     <row r="89">
-      <c r="D89" s="8"/>
+      <c r="D89" s="9"/>
     </row>
     <row r="90">
-      <c r="D90" s="8"/>
+      <c r="D90" s="9"/>
     </row>
     <row r="91">
-      <c r="D91" s="8"/>
+      <c r="D91" s="9"/>
     </row>
     <row r="92">
-      <c r="D92" s="8"/>
+      <c r="D92" s="9"/>
     </row>
     <row r="93">
-      <c r="D93" s="8"/>
+      <c r="D93" s="9"/>
     </row>
     <row r="94">
-      <c r="D94" s="8"/>
+      <c r="D94" s="9"/>
     </row>
     <row r="95">
-      <c r="D95" s="8"/>
+      <c r="D95" s="9"/>
     </row>
     <row r="96">
-      <c r="D96" s="8"/>
+      <c r="D96" s="9"/>
     </row>
     <row r="97">
-      <c r="D97" s="8"/>
+      <c r="D97" s="9"/>
     </row>
     <row r="98">
-      <c r="D98" s="8"/>
+      <c r="D98" s="9"/>
     </row>
     <row r="99">
-      <c r="D99" s="8"/>
+      <c r="D99" s="9"/>
     </row>
     <row r="100">
-      <c r="D100" s="8"/>
+      <c r="D100" s="9"/>
     </row>
     <row r="101">
-      <c r="D101" s="8"/>
+      <c r="D101" s="9"/>
     </row>
     <row r="102">
-      <c r="D102" s="8"/>
+      <c r="D102" s="9"/>
     </row>
     <row r="103">
-      <c r="D103" s="8"/>
+      <c r="D103" s="9"/>
     </row>
     <row r="104">
-      <c r="D104" s="8"/>
+      <c r="D104" s="9"/>
     </row>
     <row r="105">
-      <c r="D105" s="8"/>
+      <c r="D105" s="9"/>
     </row>
     <row r="106">
-      <c r="D106" s="8"/>
+      <c r="D106" s="9"/>
     </row>
     <row r="107">
-      <c r="D107" s="8"/>
+      <c r="D107" s="9"/>
     </row>
     <row r="108">
-      <c r="D108" s="8"/>
+      <c r="D108" s="9"/>
     </row>
     <row r="109">
-      <c r="D109" s="8"/>
+      <c r="D109" s="9"/>
     </row>
     <row r="110">
-      <c r="D110" s="8"/>
+      <c r="D110" s="9"/>
     </row>
     <row r="111">
-      <c r="D111" s="8"/>
+      <c r="D111" s="9"/>
     </row>
     <row r="112">
-      <c r="D112" s="8"/>
+      <c r="D112" s="9"/>
     </row>
     <row r="113">
-      <c r="D113" s="8"/>
+      <c r="D113" s="9"/>
     </row>
     <row r="114">
-      <c r="D114" s="8"/>
+      <c r="D114" s="9"/>
     </row>
     <row r="115">
-      <c r="D115" s="8"/>
+      <c r="D115" s="9"/>
     </row>
     <row r="116">
-      <c r="D116" s="8"/>
+      <c r="D116" s="9"/>
     </row>
     <row r="117">
-      <c r="D117" s="8"/>
+      <c r="D117" s="9"/>
     </row>
     <row r="118">
-      <c r="D118" s="8"/>
+      <c r="D118" s="9"/>
     </row>
     <row r="119">
-      <c r="D119" s="8"/>
+      <c r="D119" s="9"/>
     </row>
     <row r="120">
-      <c r="D120" s="8"/>
+      <c r="D120" s="9"/>
     </row>
     <row r="121">
-      <c r="D121" s="8"/>
+      <c r="D121" s="9"/>
     </row>
     <row r="122">
-      <c r="D122" s="8"/>
+      <c r="D122" s="9"/>
     </row>
     <row r="123">
-      <c r="D123" s="8"/>
+      <c r="D123" s="9"/>
     </row>
     <row r="124">
-      <c r="D124" s="8"/>
+      <c r="D124" s="9"/>
     </row>
     <row r="125">
-      <c r="D125" s="8"/>
+      <c r="D125" s="9"/>
     </row>
     <row r="126">
-      <c r="D126" s="8"/>
+      <c r="D126" s="9"/>
     </row>
     <row r="127">
-      <c r="D127" s="8"/>
+      <c r="D127" s="9"/>
     </row>
     <row r="128">
-      <c r="D128" s="8"/>
+      <c r="D128" s="9"/>
     </row>
     <row r="129">
-      <c r="D129" s="8"/>
+      <c r="D129" s="9"/>
     </row>
     <row r="130">
-      <c r="D130" s="8"/>
+      <c r="D130" s="9"/>
     </row>
     <row r="131">
-      <c r="D131" s="8"/>
+      <c r="D131" s="9"/>
     </row>
     <row r="132">
-      <c r="D132" s="8"/>
+      <c r="D132" s="9"/>
     </row>
     <row r="133">
-      <c r="D133" s="8"/>
+      <c r="D133" s="9"/>
     </row>
     <row r="134">
-      <c r="D134" s="8"/>
+      <c r="D134" s="9"/>
     </row>
     <row r="135">
-      <c r="D135" s="8"/>
+      <c r="D135" s="9"/>
     </row>
     <row r="136">
-      <c r="D136" s="8"/>
+      <c r="D136" s="9"/>
     </row>
     <row r="137">
-      <c r="D137" s="8"/>
+      <c r="D137" s="9"/>
     </row>
     <row r="138">
-      <c r="D138" s="8"/>
+      <c r="D138" s="9"/>
     </row>
     <row r="139">
-      <c r="D139" s="8"/>
+      <c r="D139" s="9"/>
     </row>
     <row r="140">
-      <c r="D140" s="8"/>
+      <c r="D140" s="9"/>
     </row>
     <row r="141">
-      <c r="D141" s="8"/>
+      <c r="D141" s="9"/>
     </row>
     <row r="142">
-      <c r="D142" s="8"/>
+      <c r="D142" s="9"/>
     </row>
     <row r="143">
-      <c r="D143" s="8"/>
+      <c r="D143" s="9"/>
     </row>
     <row r="144">
-      <c r="D144" s="8"/>
+      <c r="D144" s="9"/>
     </row>
     <row r="145">
-      <c r="D145" s="8"/>
+      <c r="D145" s="9"/>
     </row>
     <row r="146">
-      <c r="D146" s="8"/>
+      <c r="D146" s="9"/>
     </row>
     <row r="147">
-      <c r="D147" s="8"/>
+      <c r="D147" s="9"/>
     </row>
     <row r="148">
-      <c r="D148" s="8"/>
+      <c r="D148" s="9"/>
     </row>
     <row r="149">
-      <c r="D149" s="8"/>
+      <c r="D149" s="9"/>
     </row>
     <row r="150">
-      <c r="D150" s="8"/>
+      <c r="D150" s="9"/>
     </row>
     <row r="151">
-      <c r="D151" s="8"/>
+      <c r="D151" s="9"/>
     </row>
     <row r="152">
-      <c r="D152" s="8"/>
+      <c r="D152" s="9"/>
     </row>
     <row r="153">
-      <c r="D153" s="8"/>
+      <c r="D153" s="9"/>
     </row>
     <row r="154">
-      <c r="D154" s="8"/>
+      <c r="D154" s="9"/>
     </row>
     <row r="155">
-      <c r="D155" s="8"/>
+      <c r="D155" s="9"/>
     </row>
     <row r="156">
-      <c r="D156" s="8"/>
+      <c r="D156" s="9"/>
     </row>
     <row r="157">
-      <c r="D157" s="8"/>
+      <c r="D157" s="9"/>
     </row>
     <row r="158">
-      <c r="D158" s="8"/>
+      <c r="D158" s="9"/>
     </row>
     <row r="159">
-      <c r="D159" s="8"/>
+      <c r="D159" s="9"/>
     </row>
     <row r="160">
-      <c r="D160" s="8"/>
+      <c r="D160" s="9"/>
     </row>
     <row r="161">
-      <c r="D161" s="8"/>
+      <c r="D161" s="9"/>
     </row>
     <row r="162">
-      <c r="D162" s="8"/>
+      <c r="D162" s="9"/>
     </row>
     <row r="163">
-      <c r="D163" s="8"/>
+      <c r="D163" s="9"/>
     </row>
     <row r="164">
-      <c r="D164" s="8"/>
+      <c r="D164" s="9"/>
     </row>
     <row r="165">
-      <c r="D165" s="8"/>
+      <c r="D165" s="9"/>
     </row>
     <row r="166">
-      <c r="D166" s="8"/>
+      <c r="D166" s="9"/>
     </row>
     <row r="167">
-      <c r="D167" s="8"/>
+      <c r="D167" s="9"/>
     </row>
     <row r="168">
-      <c r="D168" s="8"/>
+      <c r="D168" s="9"/>
     </row>
     <row r="169">
-      <c r="D169" s="8"/>
+      <c r="D169" s="9"/>
     </row>
     <row r="170">
-      <c r="D170" s="8"/>
+      <c r="D170" s="9"/>
     </row>
     <row r="171">
-      <c r="D171" s="8"/>
+      <c r="D171" s="9"/>
     </row>
     <row r="172">
-      <c r="D172" s="8"/>
+      <c r="D172" s="9"/>
     </row>
     <row r="173">
-      <c r="D173" s="8"/>
+      <c r="D173" s="9"/>
     </row>
     <row r="174">
-      <c r="D174" s="8"/>
+      <c r="D174" s="9"/>
     </row>
     <row r="175">
-      <c r="D175" s="8"/>
+      <c r="D175" s="9"/>
     </row>
     <row r="176">
-      <c r="D176" s="8"/>
+      <c r="D176" s="9"/>
     </row>
     <row r="177">
-      <c r="D177" s="8"/>
+      <c r="D177" s="9"/>
     </row>
     <row r="178">
-      <c r="D178" s="8"/>
+      <c r="D178" s="9"/>
     </row>
     <row r="179">
-      <c r="D179" s="8"/>
+      <c r="D179" s="9"/>
     </row>
     <row r="180">
-      <c r="D180" s="8"/>
+      <c r="D180" s="9"/>
     </row>
     <row r="181">
-      <c r="D181" s="8"/>
+      <c r="D181" s="9"/>
     </row>
     <row r="182">
-      <c r="D182" s="8"/>
+      <c r="D182" s="9"/>
     </row>
     <row r="183">
-      <c r="D183" s="8"/>
+      <c r="D183" s="9"/>
     </row>
     <row r="184">
-      <c r="D184" s="8"/>
+      <c r="D184" s="9"/>
     </row>
     <row r="185">
-      <c r="D185" s="8"/>
+      <c r="D185" s="9"/>
     </row>
     <row r="186">
-      <c r="D186" s="8"/>
+      <c r="D186" s="9"/>
     </row>
     <row r="187">
-      <c r="D187" s="8"/>
+      <c r="D187" s="9"/>
     </row>
     <row r="188">
-      <c r="D188" s="8"/>
+      <c r="D188" s="9"/>
     </row>
     <row r="189">
-      <c r="D189" s="8"/>
+      <c r="D189" s="9"/>
     </row>
     <row r="190">
-      <c r="D190" s="8"/>
+      <c r="D190" s="9"/>
     </row>
     <row r="191">
-      <c r="D191" s="8"/>
+      <c r="D191" s="9"/>
     </row>
     <row r="192">
-      <c r="D192" s="8"/>
+      <c r="D192" s="9"/>
     </row>
     <row r="193">
-      <c r="D193" s="8"/>
+      <c r="D193" s="9"/>
     </row>
     <row r="194">
-      <c r="D194" s="8"/>
+      <c r="D194" s="9"/>
     </row>
     <row r="195">
-      <c r="D195" s="8"/>
+      <c r="D195" s="9"/>
     </row>
     <row r="196">
-      <c r="D196" s="8"/>
+      <c r="D196" s="9"/>
     </row>
     <row r="197">
-      <c r="D197" s="8"/>
+      <c r="D197" s="9"/>
     </row>
     <row r="198">
-      <c r="D198" s="8"/>
+      <c r="D198" s="9"/>
     </row>
     <row r="199">
-      <c r="D199" s="8"/>
+      <c r="D199" s="9"/>
     </row>
     <row r="200">
-      <c r="D200" s="8"/>
+      <c r="D200" s="9"/>
     </row>
     <row r="201">
-      <c r="D201" s="8"/>
+      <c r="D201" s="9"/>
     </row>
     <row r="202">
-      <c r="D202" s="8"/>
+      <c r="D202" s="9"/>
     </row>
     <row r="203">
-      <c r="D203" s="8"/>
+      <c r="D203" s="9"/>
     </row>
     <row r="204">
-      <c r="D204" s="8"/>
+      <c r="D204" s="9"/>
     </row>
     <row r="205">
-      <c r="D205" s="8"/>
+      <c r="D205" s="9"/>
     </row>
     <row r="206">
-      <c r="D206" s="8"/>
+      <c r="D206" s="9"/>
     </row>
     <row r="207">
-      <c r="D207" s="8"/>
+      <c r="D207" s="9"/>
     </row>
     <row r="208">
-      <c r="D208" s="8"/>
+      <c r="D208" s="9"/>
     </row>
     <row r="209">
-      <c r="D209" s="8"/>
+      <c r="D209" s="9"/>
     </row>
     <row r="210">
-      <c r="D210" s="8"/>
+      <c r="D210" s="9"/>
     </row>
     <row r="211">
-      <c r="D211" s="8"/>
+      <c r="D211" s="9"/>
     </row>
     <row r="212">
-      <c r="D212" s="8"/>
+      <c r="D212" s="9"/>
     </row>
     <row r="213">
-      <c r="D213" s="8"/>
+      <c r="D213" s="9"/>
     </row>
     <row r="214">
-      <c r="D214" s="8"/>
+      <c r="D214" s="9"/>
     </row>
     <row r="215">
-      <c r="D215" s="8"/>
+      <c r="D215" s="9"/>
     </row>
     <row r="216">
-      <c r="D216" s="8"/>
+      <c r="D216" s="9"/>
     </row>
     <row r="217">
-      <c r="D217" s="8"/>
+      <c r="D217" s="9"/>
     </row>
     <row r="218">
-      <c r="D218" s="8"/>
+      <c r="D218" s="9"/>
     </row>
     <row r="219">
-      <c r="D219" s="8"/>
+      <c r="D219" s="9"/>
     </row>
     <row r="220">
-      <c r="D220" s="8"/>
+      <c r="D220" s="9"/>
     </row>
     <row r="221">
-      <c r="D221" s="8"/>
+      <c r="D221" s="9"/>
     </row>
     <row r="222">
-      <c r="D222" s="8"/>
+      <c r="D222" s="9"/>
     </row>
     <row r="223">
-      <c r="D223" s="8"/>
+      <c r="D223" s="9"/>
     </row>
     <row r="224">
-      <c r="D224" s="8"/>
+      <c r="D224" s="9"/>
     </row>
     <row r="225">
-      <c r="D225" s="8"/>
+      <c r="D225" s="9"/>
     </row>
     <row r="226">
-      <c r="D226" s="8"/>
+      <c r="D226" s="9"/>
     </row>
     <row r="227">
-      <c r="D227" s="8"/>
+      <c r="D227" s="9"/>
     </row>
     <row r="228">
-      <c r="D228" s="8"/>
+      <c r="D228" s="9"/>
     </row>
     <row r="229">
-      <c r="D229" s="8"/>
+      <c r="D229" s="9"/>
     </row>
     <row r="230">
-      <c r="D230" s="8"/>
+      <c r="D230" s="9"/>
     </row>
     <row r="231">
-      <c r="D231" s="8"/>
+      <c r="D231" s="9"/>
     </row>
     <row r="232">
-      <c r="D232" s="8"/>
+      <c r="D232" s="9"/>
     </row>
     <row r="233">
-      <c r="D233" s="8"/>
+      <c r="D233" s="9"/>
     </row>
     <row r="234">
-      <c r="D234" s="8"/>
+      <c r="D234" s="9"/>
     </row>
     <row r="235">
-      <c r="D235" s="8"/>
+      <c r="D235" s="9"/>
     </row>
     <row r="236">
-      <c r="D236" s="8"/>
+      <c r="D236" s="9"/>
     </row>
     <row r="237">
-      <c r="D237" s="8"/>
+      <c r="D237" s="9"/>
     </row>
     <row r="238">
-      <c r="D238" s="8"/>
+      <c r="D238" s="9"/>
     </row>
     <row r="239">
-      <c r="D239" s="8"/>
+      <c r="D239" s="9"/>
     </row>
     <row r="240">
-      <c r="D240" s="8"/>
+      <c r="D240" s="9"/>
     </row>
     <row r="241">
-      <c r="D241" s="8"/>
+      <c r="D241" s="9"/>
     </row>
     <row r="242">
-      <c r="D242" s="8"/>
+      <c r="D242" s="9"/>
     </row>
     <row r="243">
-      <c r="D243" s="8"/>
+      <c r="D243" s="9"/>
     </row>
     <row r="244">
-      <c r="D244" s="8"/>
+      <c r="D244" s="9"/>
     </row>
     <row r="245">
-      <c r="D245" s="8"/>
+      <c r="D245" s="9"/>
     </row>
     <row r="246">
-      <c r="D246" s="8"/>
+      <c r="D246" s="9"/>
     </row>
     <row r="247">
-      <c r="D247" s="8"/>
+      <c r="D247" s="9"/>
     </row>
     <row r="248">
-      <c r="D248" s="8"/>
+      <c r="D248" s="9"/>
     </row>
     <row r="249">
-      <c r="D249" s="8"/>
+      <c r="D249" s="9"/>
     </row>
     <row r="250">
-      <c r="D250" s="8"/>
+      <c r="D250" s="9"/>
     </row>
     <row r="251">
-      <c r="D251" s="8"/>
+      <c r="D251" s="9"/>
     </row>
     <row r="252">
-      <c r="D252" s="8"/>
+      <c r="D252" s="9"/>
     </row>
     <row r="253">
-      <c r="D253" s="8"/>
+      <c r="D253" s="9"/>
     </row>
     <row r="254">
-      <c r="D254" s="8"/>
+      <c r="D254" s="9"/>
     </row>
     <row r="255">
-      <c r="D255" s="8"/>
+      <c r="D255" s="9"/>
     </row>
     <row r="256">
-      <c r="D256" s="8"/>
+      <c r="D256" s="9"/>
     </row>
     <row r="257">
-      <c r="D257" s="8"/>
+      <c r="D257" s="9"/>
     </row>
     <row r="258">
-      <c r="D258" s="8"/>
+      <c r="D258" s="9"/>
     </row>
     <row r="259">
-      <c r="D259" s="8"/>
+      <c r="D259" s="9"/>
     </row>
     <row r="260">
-      <c r="D260" s="8"/>
+      <c r="D260" s="9"/>
     </row>
     <row r="261">
-      <c r="D261" s="8"/>
+      <c r="D261" s="9"/>
     </row>
     <row r="262">
-      <c r="D262" s="8"/>
+      <c r="D262" s="9"/>
     </row>
     <row r="263">
-      <c r="D263" s="8"/>
+      <c r="D263" s="9"/>
     </row>
     <row r="264">
-      <c r="D264" s="8"/>
+      <c r="D264" s="9"/>
     </row>
     <row r="265">
-      <c r="D265" s="8"/>
+      <c r="D265" s="9"/>
     </row>
     <row r="266">
-      <c r="D266" s="8"/>
+      <c r="D266" s="9"/>
     </row>
     <row r="267">
-      <c r="D267" s="8"/>
+      <c r="D267" s="9"/>
     </row>
     <row r="268">
-      <c r="D268" s="8"/>
+      <c r="D268" s="9"/>
     </row>
     <row r="269">
-      <c r="D269" s="8"/>
+      <c r="D269" s="9"/>
     </row>
     <row r="270">
-      <c r="D270" s="8"/>
+      <c r="D270" s="9"/>
     </row>
     <row r="271">
-      <c r="D271" s="8"/>
+      <c r="D271" s="9"/>
     </row>
     <row r="272">
-      <c r="D272" s="8"/>
+      <c r="D272" s="9"/>
     </row>
     <row r="273">
-      <c r="D273" s="8"/>
+      <c r="D273" s="9"/>
     </row>
     <row r="274">
-      <c r="D274" s="8"/>
+      <c r="D274" s="9"/>
     </row>
     <row r="275">
-      <c r="D275" s="8"/>
+      <c r="D275" s="9"/>
     </row>
     <row r="276">
-      <c r="D276" s="8"/>
+      <c r="D276" s="9"/>
     </row>
     <row r="277">
-      <c r="D277" s="8"/>
+      <c r="D277" s="9"/>
     </row>
     <row r="278">
-      <c r="D278" s="8"/>
+      <c r="D278" s="9"/>
     </row>
     <row r="279">
-      <c r="D279" s="8"/>
+      <c r="D279" s="9"/>
     </row>
     <row r="280">
-      <c r="D280" s="8"/>
+      <c r="D280" s="9"/>
     </row>
     <row r="281">
-      <c r="D281" s="8"/>
+      <c r="D281" s="9"/>
     </row>
     <row r="282">
-      <c r="D282" s="8"/>
+      <c r="D282" s="9"/>
     </row>
     <row r="283">
-      <c r="D283" s="8"/>
+      <c r="D283" s="9"/>
     </row>
     <row r="284">
-      <c r="D284" s="8"/>
+      <c r="D284" s="9"/>
     </row>
     <row r="285">
-      <c r="D285" s="8"/>
+      <c r="D285" s="9"/>
     </row>
     <row r="286">
-      <c r="D286" s="8"/>
+      <c r="D286" s="9"/>
     </row>
     <row r="287">
-      <c r="D287" s="8"/>
+      <c r="D287" s="9"/>
     </row>
     <row r="288">
-      <c r="D288" s="8"/>
+      <c r="D288" s="9"/>
     </row>
     <row r="289">
-      <c r="D289" s="8"/>
+      <c r="D289" s="9"/>
     </row>
     <row r="290">
-      <c r="D290" s="8"/>
+      <c r="D290" s="9"/>
     </row>
     <row r="291">
-      <c r="D291" s="8"/>
+      <c r="D291" s="9"/>
     </row>
     <row r="292">
-      <c r="D292" s="8"/>
+      <c r="D292" s="9"/>
     </row>
     <row r="293">
-      <c r="D293" s="8"/>
+      <c r="D293" s="9"/>
     </row>
     <row r="294">
-      <c r="D294" s="8"/>
+      <c r="D294" s="9"/>
     </row>
     <row r="295">
-      <c r="D295" s="8"/>
+      <c r="D295" s="9"/>
     </row>
     <row r="296">
-      <c r="D296" s="8"/>
+      <c r="D296" s="9"/>
     </row>
     <row r="297">
-      <c r="D297" s="8"/>
+      <c r="D297" s="9"/>
     </row>
     <row r="298">
-      <c r="D298" s="8"/>
+      <c r="D298" s="9"/>
     </row>
     <row r="299">
-      <c r="D299" s="8"/>
+      <c r="D299" s="9"/>
     </row>
     <row r="300">
-      <c r="D300" s="8"/>
+      <c r="D300" s="9"/>
     </row>
     <row r="301">
-      <c r="D301" s="8"/>
+      <c r="D301" s="9"/>
     </row>
     <row r="302">
-      <c r="D302" s="8"/>
+      <c r="D302" s="9"/>
     </row>
     <row r="303">
-      <c r="D303" s="8"/>
+      <c r="D303" s="9"/>
     </row>
     <row r="304">
-      <c r="D304" s="8"/>
+      <c r="D304" s="9"/>
     </row>
     <row r="305">
-      <c r="D305" s="8"/>
+      <c r="D305" s="9"/>
     </row>
     <row r="306">
-      <c r="D306" s="8"/>
+      <c r="D306" s="9"/>
     </row>
     <row r="307">
-      <c r="D307" s="8"/>
+      <c r="D307" s="9"/>
     </row>
     <row r="308">
-      <c r="D308" s="8"/>
+      <c r="D308" s="9"/>
     </row>
     <row r="309">
-      <c r="D309" s="8"/>
+      <c r="D309" s="9"/>
     </row>
     <row r="310">
-      <c r="D310" s="8"/>
+      <c r="D310" s="9"/>
     </row>
     <row r="311">
-      <c r="D311" s="8"/>
+      <c r="D311" s="9"/>
     </row>
     <row r="312">
-      <c r="D312" s="8"/>
+      <c r="D312" s="9"/>
     </row>
     <row r="313">
-      <c r="D313" s="8"/>
+      <c r="D313" s="9"/>
     </row>
     <row r="314">
-      <c r="D314" s="8"/>
+      <c r="D314" s="9"/>
     </row>
     <row r="315">
-      <c r="D315" s="8"/>
+      <c r="D315" s="9"/>
     </row>
     <row r="316">
-      <c r="D316" s="8"/>
+      <c r="D316" s="9"/>
     </row>
     <row r="317">
-      <c r="D317" s="8"/>
+      <c r="D317" s="9"/>
     </row>
     <row r="318">
-      <c r="D318" s="8"/>
+      <c r="D318" s="9"/>
     </row>
     <row r="319">
-      <c r="D319" s="8"/>
+      <c r="D319" s="9"/>
     </row>
     <row r="320">
-      <c r="D320" s="8"/>
+      <c r="D320" s="9"/>
     </row>
     <row r="321">
-      <c r="D321" s="8"/>
+      <c r="D321" s="9"/>
     </row>
     <row r="322">
-      <c r="D322" s="8"/>
+      <c r="D322" s="9"/>
     </row>
     <row r="323">
-      <c r="D323" s="8"/>
+      <c r="D323" s="9"/>
     </row>
     <row r="324">
-      <c r="D324" s="8"/>
+      <c r="D324" s="9"/>
     </row>
     <row r="325">
-      <c r="D325" s="8"/>
+      <c r="D325" s="9"/>
     </row>
     <row r="326">
-      <c r="D326" s="8"/>
+      <c r="D326" s="9"/>
     </row>
     <row r="327">
-      <c r="D327" s="8"/>
+      <c r="D327" s="9"/>
     </row>
     <row r="328">
-      <c r="D328" s="8"/>
+      <c r="D328" s="9"/>
     </row>
     <row r="329">
-      <c r="D329" s="8"/>
+      <c r="D329" s="9"/>
     </row>
     <row r="330">
-      <c r="D330" s="8"/>
+      <c r="D330" s="9"/>
     </row>
     <row r="331">
-      <c r="D331" s="8"/>
+      <c r="D331" s="9"/>
     </row>
     <row r="332">
-      <c r="D332" s="8"/>
+      <c r="D332" s="9"/>
     </row>
     <row r="333">
-      <c r="D333" s="8"/>
+      <c r="D333" s="9"/>
     </row>
     <row r="334">
-      <c r="D334" s="8"/>
+      <c r="D334" s="9"/>
     </row>
     <row r="335">
-      <c r="D335" s="8"/>
+      <c r="D335" s="9"/>
     </row>
     <row r="336">
-      <c r="D336" s="8"/>
+      <c r="D336" s="9"/>
     </row>
     <row r="337">
-      <c r="D337" s="8"/>
+      <c r="D337" s="9"/>
     </row>
     <row r="338">
-      <c r="D338" s="8"/>
+      <c r="D338" s="9"/>
     </row>
     <row r="339">
-      <c r="D339" s="8"/>
+      <c r="D339" s="9"/>
     </row>
     <row r="340">
-      <c r="D340" s="8"/>
+      <c r="D340" s="9"/>
     </row>
     <row r="341">
-      <c r="D341" s="8"/>
+      <c r="D341" s="9"/>
     </row>
     <row r="342">
-      <c r="D342" s="8"/>
+      <c r="D342" s="9"/>
     </row>
     <row r="343">
-      <c r="D343" s="8"/>
+      <c r="D343" s="9"/>
     </row>
     <row r="344">
-      <c r="D344" s="8"/>
+      <c r="D344" s="9"/>
     </row>
     <row r="345">
-      <c r="D345" s="8"/>
+      <c r="D345" s="9"/>
     </row>
     <row r="346">
-      <c r="D346" s="8"/>
+      <c r="D346" s="9"/>
     </row>
     <row r="347">
-      <c r="D347" s="8"/>
+      <c r="D347" s="9"/>
     </row>
     <row r="348">
-      <c r="D348" s="8"/>
+      <c r="D348" s="9"/>
     </row>
     <row r="349">
-      <c r="D349" s="8"/>
+      <c r="D349" s="9"/>
     </row>
     <row r="350">
-      <c r="D350" s="8"/>
+      <c r="D350" s="9"/>
     </row>
     <row r="351">
-      <c r="D351" s="8"/>
+      <c r="D351" s="9"/>
     </row>
     <row r="352">
-      <c r="D352" s="8"/>
+      <c r="D352" s="9"/>
     </row>
     <row r="353">
-      <c r="D353" s="8"/>
+      <c r="D353" s="9"/>
     </row>
     <row r="354">
-      <c r="D354" s="8"/>
+      <c r="D354" s="9"/>
     </row>
     <row r="355">
-      <c r="D355" s="8"/>
+      <c r="D355" s="9"/>
     </row>
     <row r="356">
-      <c r="D356" s="8"/>
+      <c r="D356" s="9"/>
     </row>
     <row r="357">
-      <c r="D357" s="8"/>
+      <c r="D357" s="9"/>
     </row>
     <row r="358">
-      <c r="D358" s="8"/>
+      <c r="D358" s="9"/>
     </row>
     <row r="359">
-      <c r="D359" s="8"/>
+      <c r="D359" s="9"/>
     </row>
     <row r="360">
-      <c r="D360" s="8"/>
+      <c r="D360" s="9"/>
     </row>
     <row r="361">
-      <c r="D361" s="8"/>
+      <c r="D361" s="9"/>
     </row>
     <row r="362">
-      <c r="D362" s="8"/>
+      <c r="D362" s="9"/>
     </row>
     <row r="363">
-      <c r="D363" s="8"/>
+      <c r="D363" s="9"/>
     </row>
     <row r="364">
-      <c r="D364" s="8"/>
+      <c r="D364" s="9"/>
     </row>
     <row r="365">
-      <c r="D365" s="8"/>
+      <c r="D365" s="9"/>
     </row>
     <row r="366">
-      <c r="D366" s="8"/>
+      <c r="D366" s="9"/>
     </row>
     <row r="367">
-      <c r="D367" s="8"/>
+      <c r="D367" s="9"/>
     </row>
     <row r="368">
-      <c r="D368" s="8"/>
+      <c r="D368" s="9"/>
     </row>
     <row r="369">
-      <c r="D369" s="8"/>
+      <c r="D369" s="9"/>
     </row>
     <row r="370">
-      <c r="D370" s="8"/>
+      <c r="D370" s="9"/>
     </row>
     <row r="371">
-      <c r="D371" s="8"/>
+      <c r="D371" s="9"/>
     </row>
     <row r="372">
-      <c r="D372" s="8"/>
+      <c r="D372" s="9"/>
     </row>
     <row r="373">
-      <c r="D373" s="8"/>
+      <c r="D373" s="9"/>
     </row>
     <row r="374">
-      <c r="D374" s="8"/>
+      <c r="D374" s="9"/>
     </row>
     <row r="375">
-      <c r="D375" s="8"/>
+      <c r="D375" s="9"/>
     </row>
     <row r="376">
-      <c r="D376" s="8"/>
+      <c r="D376" s="9"/>
     </row>
     <row r="377">
-      <c r="D377" s="8"/>
+      <c r="D377" s="9"/>
     </row>
     <row r="378">
-      <c r="D378" s="8"/>
+      <c r="D378" s="9"/>
     </row>
     <row r="379">
-      <c r="D379" s="8"/>
+      <c r="D379" s="9"/>
     </row>
     <row r="380">
-      <c r="D380" s="8"/>
+      <c r="D380" s="9"/>
     </row>
     <row r="381">
-      <c r="D381" s="8"/>
+      <c r="D381" s="9"/>
     </row>
     <row r="382">
-      <c r="D382" s="8"/>
+      <c r="D382" s="9"/>
     </row>
     <row r="383">
-      <c r="D383" s="8"/>
+      <c r="D383" s="9"/>
     </row>
     <row r="384">
-      <c r="D384" s="8"/>
+      <c r="D384" s="9"/>
     </row>
     <row r="385">
-      <c r="D385" s="8"/>
+      <c r="D385" s="9"/>
     </row>
     <row r="386">
-      <c r="D386" s="8"/>
+      <c r="D386" s="9"/>
     </row>
     <row r="387">
-      <c r="D387" s="8"/>
+      <c r="D387" s="9"/>
     </row>
     <row r="388">
-      <c r="D388" s="8"/>
+      <c r="D388" s="9"/>
     </row>
     <row r="389">
-      <c r="D389" s="8"/>
+      <c r="D389" s="9"/>
     </row>
     <row r="390">
-      <c r="D390" s="8"/>
+      <c r="D390" s="9"/>
     </row>
     <row r="391">
-      <c r="D391" s="8"/>
+      <c r="D391" s="9"/>
     </row>
     <row r="392">
-      <c r="D392" s="8"/>
+      <c r="D392" s="9"/>
     </row>
     <row r="393">
-      <c r="D393" s="8"/>
+      <c r="D393" s="9"/>
     </row>
     <row r="394">
-      <c r="D394" s="8"/>
+      <c r="D394" s="9"/>
     </row>
     <row r="395">
-      <c r="D395" s="8"/>
+      <c r="D395" s="9"/>
     </row>
     <row r="396">
-      <c r="D396" s="8"/>
+      <c r="D396" s="9"/>
     </row>
     <row r="397">
-      <c r="D397" s="8"/>
+      <c r="D397" s="9"/>
     </row>
     <row r="398">
-      <c r="D398" s="8"/>
+      <c r="D398" s="9"/>
     </row>
     <row r="399">
-      <c r="D399" s="8"/>
+      <c r="D399" s="9"/>
     </row>
     <row r="400">
-      <c r="D400" s="8"/>
+      <c r="D400" s="9"/>
     </row>
     <row r="401">
-      <c r="D401" s="8"/>
+      <c r="D401" s="9"/>
     </row>
     <row r="402">
-      <c r="D402" s="8"/>
+      <c r="D402" s="9"/>
     </row>
     <row r="403">
-      <c r="D403" s="8"/>
+      <c r="D403" s="9"/>
     </row>
     <row r="404">
-      <c r="D404" s="8"/>
+      <c r="D404" s="9"/>
     </row>
     <row r="405">
-      <c r="D405" s="8"/>
+      <c r="D405" s="9"/>
     </row>
     <row r="406">
-      <c r="D406" s="8"/>
+      <c r="D406" s="9"/>
     </row>
     <row r="407">
-      <c r="D407" s="8"/>
+      <c r="D407" s="9"/>
     </row>
     <row r="408">
-      <c r="D408" s="8"/>
+      <c r="D408" s="9"/>
     </row>
     <row r="409">
-      <c r="D409" s="8"/>
+      <c r="D409" s="9"/>
     </row>
     <row r="410">
-      <c r="D410" s="8"/>
+      <c r="D410" s="9"/>
     </row>
     <row r="411">
-      <c r="D411" s="8"/>
+      <c r="D411" s="9"/>
     </row>
     <row r="412">
-      <c r="D412" s="8"/>
+      <c r="D412" s="9"/>
     </row>
     <row r="413">
-      <c r="D413" s="8"/>
+      <c r="D413" s="9"/>
     </row>
     <row r="414">
-      <c r="D414" s="8"/>
+      <c r="D414" s="9"/>
     </row>
     <row r="415">
-      <c r="D415" s="8"/>
+      <c r="D415" s="9"/>
     </row>
     <row r="416">
-      <c r="D416" s="8"/>
+      <c r="D416" s="9"/>
     </row>
     <row r="417">
-      <c r="D417" s="8"/>
+      <c r="D417" s="9"/>
     </row>
     <row r="418">
-      <c r="D418" s="8"/>
+      <c r="D418" s="9"/>
     </row>
     <row r="419">
-      <c r="D419" s="8"/>
+      <c r="D419" s="9"/>
     </row>
     <row r="420">
-      <c r="D420" s="8"/>
+      <c r="D420" s="9"/>
     </row>
     <row r="421">
-      <c r="D421" s="8"/>
+      <c r="D421" s="9"/>
     </row>
     <row r="422">
-      <c r="D422" s="8"/>
+      <c r="D422" s="9"/>
     </row>
     <row r="423">
-      <c r="D423" s="8"/>
+      <c r="D423" s="9"/>
     </row>
     <row r="424">
-      <c r="D424" s="8"/>
+      <c r="D424" s="9"/>
     </row>
     <row r="425">
-      <c r="D425" s="8"/>
+      <c r="D425" s="9"/>
     </row>
     <row r="426">
-      <c r="D426" s="8"/>
+      <c r="D426" s="9"/>
     </row>
     <row r="427">
-      <c r="D427" s="8"/>
+      <c r="D427" s="9"/>
     </row>
     <row r="428">
-      <c r="D428" s="8"/>
+      <c r="D428" s="9"/>
     </row>
     <row r="429">
-      <c r="D429" s="8"/>
+      <c r="D429" s="9"/>
     </row>
     <row r="430">
-      <c r="D430" s="8"/>
+      <c r="D430" s="9"/>
     </row>
     <row r="431">
-      <c r="D431" s="8"/>
+      <c r="D431" s="9"/>
     </row>
     <row r="432">
-      <c r="D432" s="8"/>
+      <c r="D432" s="9"/>
     </row>
     <row r="433">
-      <c r="D433" s="8"/>
+      <c r="D433" s="9"/>
     </row>
     <row r="434">
-      <c r="D434" s="8"/>
+      <c r="D434" s="9"/>
     </row>
     <row r="435">
-      <c r="D435" s="8"/>
+      <c r="D435" s="9"/>
     </row>
     <row r="436">
-      <c r="D436" s="8"/>
+      <c r="D436" s="9"/>
     </row>
     <row r="437">
-      <c r="D437" s="8"/>
+      <c r="D437" s="9"/>
     </row>
     <row r="438">
-      <c r="D438" s="8"/>
+      <c r="D438" s="9"/>
     </row>
     <row r="439">
-      <c r="D439" s="8"/>
+      <c r="D439" s="9"/>
     </row>
     <row r="440">
-      <c r="D440" s="8"/>
+      <c r="D440" s="9"/>
     </row>
     <row r="441">
-      <c r="D441" s="8"/>
+      <c r="D441" s="9"/>
     </row>
     <row r="442">
-      <c r="D442" s="8"/>
+      <c r="D442" s="9"/>
     </row>
     <row r="443">
-      <c r="D443" s="8"/>
+      <c r="D443" s="9"/>
     </row>
     <row r="444">
-      <c r="D444" s="8"/>
+      <c r="D444" s="9"/>
     </row>
     <row r="445">
-      <c r="D445" s="8"/>
+      <c r="D445" s="9"/>
     </row>
     <row r="446">
-      <c r="D446" s="8"/>
+      <c r="D446" s="9"/>
     </row>
     <row r="447">
-      <c r="D447" s="8"/>
+      <c r="D447" s="9"/>
     </row>
     <row r="448">
-      <c r="D448" s="8"/>
+      <c r="D448" s="9"/>
     </row>
     <row r="449">
-      <c r="D449" s="8"/>
+      <c r="D449" s="9"/>
     </row>
     <row r="450">
-      <c r="D450" s="8"/>
+      <c r="D450" s="9"/>
     </row>
     <row r="451">
-      <c r="D451" s="8"/>
+      <c r="D451" s="9"/>
     </row>
     <row r="452">
-      <c r="D452" s="8"/>
+      <c r="D452" s="9"/>
     </row>
     <row r="453">
-      <c r="D453" s="8"/>
+      <c r="D453" s="9"/>
     </row>
     <row r="454">
-      <c r="D454" s="8"/>
+      <c r="D454" s="9"/>
     </row>
     <row r="455">
-      <c r="D455" s="8"/>
+      <c r="D455" s="9"/>
     </row>
     <row r="456">
-      <c r="D456" s="8"/>
+      <c r="D456" s="9"/>
     </row>
     <row r="457">
-      <c r="D457" s="8"/>
+      <c r="D457" s="9"/>
     </row>
     <row r="458">
-      <c r="D458" s="8"/>
+      <c r="D458" s="9"/>
     </row>
     <row r="459">
-      <c r="D459" s="8"/>
+      <c r="D459" s="9"/>
     </row>
     <row r="460">
-      <c r="D460" s="8"/>
+      <c r="D460" s="9"/>
     </row>
     <row r="461">
-      <c r="D461" s="8"/>
+      <c r="D461" s="9"/>
     </row>
     <row r="462">
-      <c r="D462" s="8"/>
+      <c r="D462" s="9"/>
     </row>
     <row r="463">
-      <c r="D463" s="8"/>
+      <c r="D463" s="9"/>
     </row>
     <row r="464">
-      <c r="D464" s="8"/>
+      <c r="D464" s="9"/>
     </row>
     <row r="465">
-      <c r="D465" s="8"/>
+      <c r="D465" s="9"/>
     </row>
     <row r="466">
-      <c r="D466" s="8"/>
+      <c r="D466" s="9"/>
     </row>
     <row r="467">
-      <c r="D467" s="8"/>
+      <c r="D467" s="9"/>
     </row>
     <row r="468">
-      <c r="D468" s="8"/>
+      <c r="D468" s="9"/>
     </row>
     <row r="469">
-      <c r="D469" s="8"/>
+      <c r="D469" s="9"/>
     </row>
     <row r="470">
-      <c r="D470" s="8"/>
+      <c r="D470" s="9"/>
     </row>
     <row r="471">
-      <c r="D471" s="8"/>
+      <c r="D471" s="9"/>
     </row>
     <row r="472">
-      <c r="D472" s="8"/>
+      <c r="D472" s="9"/>
     </row>
     <row r="473">
-      <c r="D473" s="8"/>
+      <c r="D473" s="9"/>
     </row>
     <row r="474">
-      <c r="D474" s="8"/>
+      <c r="D474" s="9"/>
     </row>
     <row r="475">
-      <c r="D475" s="8"/>
+      <c r="D475" s="9"/>
     </row>
     <row r="476">
-      <c r="D476" s="8"/>
+      <c r="D476" s="9"/>
     </row>
     <row r="477">
-      <c r="D477" s="8"/>
+      <c r="D477" s="9"/>
     </row>
     <row r="478">
-      <c r="D478" s="8"/>
+      <c r="D478" s="9"/>
     </row>
     <row r="479">
-      <c r="D479" s="8"/>
+      <c r="D479" s="9"/>
     </row>
     <row r="480">
-      <c r="D480" s="8"/>
+      <c r="D480" s="9"/>
     </row>
     <row r="481">
-      <c r="D481" s="8"/>
+      <c r="D481" s="9"/>
     </row>
     <row r="482">
-      <c r="D482" s="8"/>
+      <c r="D482" s="9"/>
     </row>
     <row r="483">
-      <c r="D483" s="8"/>
+      <c r="D483" s="9"/>
     </row>
     <row r="484">
-      <c r="D484" s="8"/>
+      <c r="D484" s="9"/>
     </row>
     <row r="485">
-      <c r="D485" s="8"/>
+      <c r="D485" s="9"/>
     </row>
     <row r="486">
-      <c r="D486" s="8"/>
+      <c r="D486" s="9"/>
     </row>
     <row r="487">
-      <c r="D487" s="8"/>
+      <c r="D487" s="9"/>
     </row>
     <row r="488">
-      <c r="D488" s="8"/>
+      <c r="D488" s="9"/>
     </row>
     <row r="489">
-      <c r="D489" s="8"/>
+      <c r="D489" s="9"/>
     </row>
     <row r="490">
-      <c r="D490" s="8"/>
+      <c r="D490" s="9"/>
     </row>
     <row r="491">
-      <c r="D491" s="8"/>
+      <c r="D491" s="9"/>
     </row>
     <row r="492">
-      <c r="D492" s="8"/>
+      <c r="D492" s="9"/>
     </row>
     <row r="493">
-      <c r="D493" s="8"/>
+      <c r="D493" s="9"/>
     </row>
     <row r="494">
-      <c r="D494" s="8"/>
+      <c r="D494" s="9"/>
     </row>
     <row r="495">
-      <c r="D495" s="8"/>
+      <c r="D495" s="9"/>
     </row>
     <row r="496">
-      <c r="D496" s="8"/>
+      <c r="D496" s="9"/>
     </row>
     <row r="497">
-      <c r="D497" s="8"/>
+      <c r="D497" s="9"/>
     </row>
     <row r="498">
-      <c r="D498" s="8"/>
+      <c r="D498" s="9"/>
     </row>
     <row r="499">
-      <c r="D499" s="8"/>
+      <c r="D499" s="9"/>
     </row>
     <row r="500">
-      <c r="D500" s="8"/>
+      <c r="D500" s="9"/>
     </row>
     <row r="501">
-      <c r="D501" s="8"/>
+      <c r="D501" s="9"/>
     </row>
     <row r="502">
-      <c r="D502" s="8"/>
+      <c r="D502" s="9"/>
     </row>
     <row r="503">
-      <c r="D503" s="8"/>
+      <c r="D503" s="9"/>
     </row>
     <row r="504">
-      <c r="D504" s="8"/>
+      <c r="D504" s="9"/>
     </row>
     <row r="505">
-      <c r="D505" s="8"/>
+      <c r="D505" s="9"/>
     </row>
     <row r="506">
-      <c r="D506" s="8"/>
+      <c r="D506" s="9"/>
     </row>
     <row r="507">
-      <c r="D507" s="8"/>
+      <c r="D507" s="9"/>
     </row>
     <row r="508">
-      <c r="D508" s="8"/>
+      <c r="D508" s="9"/>
     </row>
     <row r="509">
-      <c r="D509" s="8"/>
+      <c r="D509" s="9"/>
     </row>
     <row r="510">
-      <c r="D510" s="8"/>
+      <c r="D510" s="9"/>
     </row>
     <row r="511">
-      <c r="D511" s="8"/>
+      <c r="D511" s="9"/>
     </row>
     <row r="512">
-      <c r="D512" s="8"/>
+      <c r="D512" s="9"/>
     </row>
     <row r="513">
-      <c r="D513" s="8"/>
+      <c r="D513" s="9"/>
     </row>
     <row r="514">
-      <c r="D514" s="8"/>
+      <c r="D514" s="9"/>
     </row>
     <row r="515">
-      <c r="D515" s="8"/>
+      <c r="D515" s="9"/>
     </row>
     <row r="516">
-      <c r="D516" s="8"/>
+      <c r="D516" s="9"/>
     </row>
     <row r="517">
-      <c r="D517" s="8"/>
+      <c r="D517" s="9"/>
     </row>
     <row r="518">
-      <c r="D518" s="8"/>
+      <c r="D518" s="9"/>
     </row>
     <row r="519">
-      <c r="D519" s="8"/>
+      <c r="D519" s="9"/>
     </row>
     <row r="520">
-      <c r="D520" s="8"/>
+      <c r="D520" s="9"/>
     </row>
     <row r="521">
-      <c r="D521" s="8"/>
+      <c r="D521" s="9"/>
     </row>
     <row r="522">
-      <c r="D522" s="8"/>
+      <c r="D522" s="9"/>
     </row>
     <row r="523">
-      <c r="D523" s="8"/>
+      <c r="D523" s="9"/>
     </row>
     <row r="524">
-      <c r="D524" s="8"/>
+      <c r="D524" s="9"/>
     </row>
     <row r="525">
-      <c r="D525" s="8"/>
+      <c r="D525" s="9"/>
     </row>
     <row r="526">
-      <c r="D526" s="8"/>
+      <c r="D526" s="9"/>
     </row>
     <row r="527">
-      <c r="D527" s="8"/>
+      <c r="D527" s="9"/>
     </row>
     <row r="528">
-      <c r="D528" s="8"/>
+      <c r="D528" s="9"/>
     </row>
     <row r="529">
-      <c r="D529" s="8"/>
+      <c r="D529" s="9"/>
     </row>
     <row r="530">
-      <c r="D530" s="8"/>
+      <c r="D530" s="9"/>
     </row>
     <row r="531">
-      <c r="D531" s="8"/>
+      <c r="D531" s="9"/>
     </row>
     <row r="532">
-      <c r="D532" s="8"/>
+      <c r="D532" s="9"/>
     </row>
     <row r="533">
-      <c r="D533" s="8"/>
+      <c r="D533" s="9"/>
     </row>
     <row r="534">
-      <c r="D534" s="8"/>
+      <c r="D534" s="9"/>
     </row>
     <row r="535">
-      <c r="D535" s="8"/>
+      <c r="D535" s="9"/>
     </row>
     <row r="536">
-      <c r="D536" s="8"/>
+      <c r="D536" s="9"/>
     </row>
     <row r="537">
-      <c r="D537" s="8"/>
+      <c r="D537" s="9"/>
     </row>
     <row r="538">
-      <c r="D538" s="8"/>
+      <c r="D538" s="9"/>
     </row>
     <row r="539">
-      <c r="D539" s="8"/>
+      <c r="D539" s="9"/>
     </row>
     <row r="540">
-      <c r="D540" s="8"/>
+      <c r="D540" s="9"/>
     </row>
     <row r="541">
-      <c r="D541" s="8"/>
+      <c r="D541" s="9"/>
     </row>
     <row r="542">
-      <c r="D542" s="8"/>
+      <c r="D542" s="9"/>
     </row>
     <row r="543">
-      <c r="D543" s="8"/>
+      <c r="D543" s="9"/>
     </row>
     <row r="544">
-      <c r="D544" s="8"/>
+      <c r="D544" s="9"/>
     </row>
     <row r="545">
-      <c r="D545" s="8"/>
+      <c r="D545" s="9"/>
     </row>
     <row r="546">
-      <c r="D546" s="8"/>
+      <c r="D546" s="9"/>
     </row>
     <row r="547">
-      <c r="D547" s="8"/>
+      <c r="D547" s="9"/>
     </row>
     <row r="548">
-      <c r="D548" s="8"/>
+      <c r="D548" s="9"/>
     </row>
     <row r="549">
-      <c r="D549" s="8"/>
+      <c r="D549" s="9"/>
     </row>
     <row r="550">
-      <c r="D550" s="8"/>
+      <c r="D550" s="9"/>
     </row>
     <row r="551">
-      <c r="D551" s="8"/>
+      <c r="D551" s="9"/>
     </row>
     <row r="552">
-      <c r="D552" s="8"/>
+      <c r="D552" s="9"/>
     </row>
     <row r="553">
-      <c r="D553" s="8"/>
+      <c r="D553" s="9"/>
     </row>
     <row r="554">
-      <c r="D554" s="8"/>
+      <c r="D554" s="9"/>
     </row>
     <row r="555">
-      <c r="D555" s="8"/>
+      <c r="D555" s="9"/>
     </row>
     <row r="556">
-      <c r="D556" s="8"/>
+      <c r="D556" s="9"/>
     </row>
     <row r="557">
-      <c r="D557" s="8"/>
+      <c r="D557" s="9"/>
     </row>
     <row r="558">
-      <c r="D558" s="8"/>
+      <c r="D558" s="9"/>
     </row>
     <row r="559">
-      <c r="D559" s="8"/>
+      <c r="D559" s="9"/>
     </row>
     <row r="560">
-      <c r="D560" s="8"/>
+      <c r="D560" s="9"/>
     </row>
     <row r="561">
-      <c r="D561" s="8"/>
+      <c r="D561" s="9"/>
     </row>
     <row r="562">
-      <c r="D562" s="8"/>
+      <c r="D562" s="9"/>
     </row>
     <row r="563">
-      <c r="D563" s="8"/>
+      <c r="D563" s="9"/>
     </row>
     <row r="564">
-      <c r="D564" s="8"/>
+      <c r="D564" s="9"/>
     </row>
     <row r="565">
-      <c r="D565" s="8"/>
+      <c r="D565" s="9"/>
     </row>
     <row r="566">
-      <c r="D566" s="8"/>
+      <c r="D566" s="9"/>
     </row>
     <row r="567">
-      <c r="D567" s="8"/>
+      <c r="D567" s="9"/>
     </row>
     <row r="568">
-      <c r="D568" s="8"/>
+      <c r="D568" s="9"/>
     </row>
     <row r="569">
-      <c r="D569" s="8"/>
+      <c r="D569" s="9"/>
     </row>
     <row r="570">
-      <c r="D570" s="8"/>
+      <c r="D570" s="9"/>
     </row>
     <row r="571">
-      <c r="D571" s="8"/>
+      <c r="D571" s="9"/>
     </row>
     <row r="572">
-      <c r="D572" s="8"/>
+      <c r="D572" s="9"/>
     </row>
     <row r="573">
-      <c r="D573" s="8"/>
+      <c r="D573" s="9"/>
     </row>
     <row r="574">
-      <c r="D574" s="8"/>
+      <c r="D574" s="9"/>
     </row>
     <row r="575">
-      <c r="D575" s="8"/>
+      <c r="D575" s="9"/>
     </row>
     <row r="576">
-      <c r="D576" s="8"/>
+      <c r="D576" s="9"/>
     </row>
     <row r="577">
-      <c r="D577" s="8"/>
+      <c r="D577" s="9"/>
     </row>
     <row r="578">
-      <c r="D578" s="8"/>
+      <c r="D578" s="9"/>
     </row>
     <row r="579">
-      <c r="D579" s="8"/>
+      <c r="D579" s="9"/>
     </row>
     <row r="580">
-      <c r="D580" s="8"/>
+      <c r="D580" s="9"/>
     </row>
     <row r="581">
-      <c r="D581" s="8"/>
+      <c r="D581" s="9"/>
     </row>
     <row r="582">
-      <c r="D582" s="8"/>
+      <c r="D582" s="9"/>
     </row>
     <row r="583">
-      <c r="D583" s="8"/>
+      <c r="D583" s="9"/>
     </row>
     <row r="584">
-      <c r="D584" s="8"/>
+      <c r="D584" s="9"/>
     </row>
     <row r="585">
-      <c r="D585" s="8"/>
+      <c r="D585" s="9"/>
     </row>
     <row r="586">
-      <c r="D586" s="8"/>
+      <c r="D586" s="9"/>
     </row>
     <row r="587">
-      <c r="D587" s="8"/>
+      <c r="D587" s="9"/>
     </row>
     <row r="588">
-      <c r="D588" s="8"/>
+      <c r="D588" s="9"/>
     </row>
     <row r="589">
-      <c r="D589" s="8"/>
+      <c r="D589" s="9"/>
     </row>
     <row r="590">
-      <c r="D590" s="8"/>
+      <c r="D590" s="9"/>
     </row>
     <row r="591">
-      <c r="D591" s="8"/>
+      <c r="D591" s="9"/>
     </row>
     <row r="592">
-      <c r="D592" s="8"/>
+      <c r="D592" s="9"/>
     </row>
     <row r="593">
-      <c r="D593" s="8"/>
+      <c r="D593" s="9"/>
     </row>
     <row r="594">
-      <c r="D594" s="8"/>
+      <c r="D594" s="9"/>
     </row>
     <row r="595">
-      <c r="D595" s="8"/>
+      <c r="D595" s="9"/>
     </row>
     <row r="596">
-      <c r="D596" s="8"/>
+      <c r="D596" s="9"/>
     </row>
     <row r="597">
-      <c r="D597" s="8"/>
+      <c r="D597" s="9"/>
     </row>
     <row r="598">
-      <c r="D598" s="8"/>
+      <c r="D598" s="9"/>
     </row>
     <row r="599">
-      <c r="D599" s="8"/>
+      <c r="D599" s="9"/>
     </row>
     <row r="600">
-      <c r="D600" s="8"/>
+      <c r="D600" s="9"/>
     </row>
     <row r="601">
-      <c r="D601" s="8"/>
+      <c r="D601" s="9"/>
     </row>
     <row r="602">
-      <c r="D602" s="8"/>
+      <c r="D602" s="9"/>
     </row>
     <row r="603">
-      <c r="D603" s="8"/>
+      <c r="D603" s="9"/>
     </row>
     <row r="604">
-      <c r="D604" s="8"/>
+      <c r="D604" s="9"/>
     </row>
     <row r="605">
-      <c r="D605" s="8"/>
+      <c r="D605" s="9"/>
     </row>
     <row r="606">
-      <c r="D606" s="8"/>
+      <c r="D606" s="9"/>
     </row>
     <row r="607">
-      <c r="D607" s="8"/>
+      <c r="D607" s="9"/>
     </row>
     <row r="608">
-      <c r="D608" s="8"/>
+      <c r="D608" s="9"/>
     </row>
     <row r="609">
-      <c r="D609" s="8"/>
+      <c r="D609" s="9"/>
     </row>
     <row r="610">
-      <c r="D610" s="8"/>
+      <c r="D610" s="9"/>
     </row>
     <row r="611">
-      <c r="D611" s="8"/>
+      <c r="D611" s="9"/>
     </row>
     <row r="612">
-      <c r="D612" s="8"/>
+      <c r="D612" s="9"/>
     </row>
     <row r="613">
-      <c r="D613" s="8"/>
+      <c r="D613" s="9"/>
     </row>
     <row r="614">
-      <c r="D614" s="8"/>
+      <c r="D614" s="9"/>
     </row>
     <row r="615">
-      <c r="D615" s="8"/>
+      <c r="D615" s="9"/>
     </row>
     <row r="616">
-      <c r="D616" s="8"/>
+      <c r="D616" s="9"/>
     </row>
     <row r="617">
-      <c r="D617" s="8"/>
+      <c r="D617" s="9"/>
     </row>
     <row r="618">
-      <c r="D618" s="8"/>
+      <c r="D618" s="9"/>
     </row>
     <row r="619">
-      <c r="D619" s="8"/>
+      <c r="D619" s="9"/>
     </row>
     <row r="620">
-      <c r="D620" s="8"/>
+      <c r="D620" s="9"/>
     </row>
     <row r="621">
-      <c r="D621" s="8"/>
+      <c r="D621" s="9"/>
     </row>
     <row r="622">
-      <c r="D622" s="8"/>
+      <c r="D622" s="9"/>
     </row>
     <row r="623">
-      <c r="D623" s="8"/>
+      <c r="D623" s="9"/>
     </row>
     <row r="624">
-      <c r="D624" s="8"/>
+      <c r="D624" s="9"/>
     </row>
     <row r="625">
-      <c r="D625" s="8"/>
+      <c r="D625" s="9"/>
     </row>
     <row r="626">
-      <c r="D626" s="8"/>
+      <c r="D626" s="9"/>
     </row>
     <row r="627">
-      <c r="D627" s="8"/>
+      <c r="D627" s="9"/>
     </row>
     <row r="628">
-      <c r="D628" s="8"/>
+      <c r="D628" s="9"/>
     </row>
     <row r="629">
-      <c r="D629" s="8"/>
+      <c r="D629" s="9"/>
     </row>
     <row r="630">
-      <c r="D630" s="8"/>
+      <c r="D630" s="9"/>
     </row>
     <row r="631">
-      <c r="D631" s="8"/>
+      <c r="D631" s="9"/>
     </row>
     <row r="632">
-      <c r="D632" s="8"/>
+      <c r="D632" s="9"/>
     </row>
     <row r="633">
-      <c r="D633" s="8"/>
+      <c r="D633" s="9"/>
     </row>
     <row r="634">
-      <c r="D634" s="8"/>
+      <c r="D634" s="9"/>
     </row>
     <row r="635">
-      <c r="D635" s="8"/>
+      <c r="D635" s="9"/>
     </row>
     <row r="636">
-      <c r="D636" s="8"/>
+      <c r="D636" s="9"/>
     </row>
     <row r="637">
-      <c r="D637" s="8"/>
+      <c r="D637" s="9"/>
     </row>
     <row r="638">
-      <c r="D638" s="8"/>
+      <c r="D638" s="9"/>
     </row>
     <row r="639">
-      <c r="D639" s="8"/>
+      <c r="D639" s="9"/>
     </row>
     <row r="640">
-      <c r="D640" s="8"/>
+      <c r="D640" s="9"/>
     </row>
     <row r="641">
-      <c r="D641" s="8"/>
+      <c r="D641" s="9"/>
     </row>
     <row r="642">
-      <c r="D642" s="8"/>
+      <c r="D642" s="9"/>
     </row>
     <row r="643">
-      <c r="D643" s="8"/>
+      <c r="D643" s="9"/>
     </row>
     <row r="644">
-      <c r="D644" s="8"/>
+      <c r="D644" s="9"/>
     </row>
     <row r="645">
-      <c r="D645" s="8"/>
+      <c r="D645" s="9"/>
     </row>
     <row r="646">
-      <c r="D646" s="8"/>
+      <c r="D646" s="9"/>
     </row>
     <row r="647">
-      <c r="D647" s="8"/>
+      <c r="D647" s="9"/>
     </row>
     <row r="648">
-      <c r="D648" s="8"/>
+      <c r="D648" s="9"/>
     </row>
     <row r="649">
-      <c r="D649" s="8"/>
+      <c r="D649" s="9"/>
     </row>
     <row r="650">
-      <c r="D650" s="8"/>
+      <c r="D650" s="9"/>
     </row>
     <row r="651">
-      <c r="D651" s="8"/>
+      <c r="D651" s="9"/>
     </row>
     <row r="652">
-      <c r="D652" s="8"/>
+      <c r="D652" s="9"/>
     </row>
     <row r="653">
-      <c r="D653" s="8"/>
+      <c r="D653" s="9"/>
     </row>
     <row r="654">
-      <c r="D654" s="8"/>
+      <c r="D654" s="9"/>
     </row>
     <row r="655">
-      <c r="D655" s="8"/>
+      <c r="D655" s="9"/>
     </row>
     <row r="656">
-      <c r="D656" s="8"/>
+      <c r="D656" s="9"/>
     </row>
     <row r="657">
-      <c r="D657" s="8"/>
+      <c r="D657" s="9"/>
     </row>
     <row r="658">
-      <c r="D658" s="8"/>
+      <c r="D658" s="9"/>
     </row>
     <row r="659">
-      <c r="D659" s="8"/>
+      <c r="D659" s="9"/>
     </row>
     <row r="660">
-      <c r="D660" s="8"/>
+      <c r="D660" s="9"/>
     </row>
     <row r="661">
-      <c r="D661" s="8"/>
+      <c r="D661" s="9"/>
     </row>
     <row r="662">
-      <c r="D662" s="8"/>
+      <c r="D662" s="9"/>
     </row>
     <row r="663">
-      <c r="D663" s="8"/>
+      <c r="D663" s="9"/>
     </row>
     <row r="664">
-      <c r="D664" s="8"/>
+      <c r="D664" s="9"/>
     </row>
     <row r="665">
-      <c r="D665" s="8"/>
+      <c r="D665" s="9"/>
     </row>
     <row r="666">
-      <c r="D666" s="8"/>
+      <c r="D666" s="9"/>
     </row>
     <row r="667">
-      <c r="D667" s="8"/>
+      <c r="D667" s="9"/>
     </row>
     <row r="668">
-      <c r="D668" s="8"/>
+      <c r="D668" s="9"/>
     </row>
     <row r="669">
-      <c r="D669" s="8"/>
+      <c r="D669" s="9"/>
     </row>
     <row r="670">
-      <c r="D670" s="8"/>
+      <c r="D670" s="9"/>
     </row>
     <row r="671">
-      <c r="D671" s="8"/>
+      <c r="D671" s="9"/>
     </row>
     <row r="672">
-      <c r="D672" s="8"/>
+      <c r="D672" s="9"/>
     </row>
     <row r="673">
-      <c r="D673" s="8"/>
+      <c r="D673" s="9"/>
     </row>
     <row r="674">
-      <c r="D674" s="8"/>
+      <c r="D674" s="9"/>
     </row>
     <row r="675">
-      <c r="D675" s="8"/>
+      <c r="D675" s="9"/>
     </row>
     <row r="676">
-      <c r="D676" s="8"/>
+      <c r="D676" s="9"/>
     </row>
     <row r="677">
-      <c r="D677" s="8"/>
+      <c r="D677" s="9"/>
     </row>
     <row r="678">
-      <c r="D678" s="8"/>
+      <c r="D678" s="9"/>
     </row>
     <row r="679">
-      <c r="D679" s="8"/>
+      <c r="D679" s="9"/>
     </row>
     <row r="680">
-      <c r="D680" s="8"/>
+      <c r="D680" s="9"/>
     </row>
     <row r="681">
-      <c r="D681" s="8"/>
+      <c r="D681" s="9"/>
     </row>
     <row r="682">
-      <c r="D682" s="8"/>
+      <c r="D682" s="9"/>
     </row>
     <row r="683">
-      <c r="D683" s="8"/>
+      <c r="D683" s="9"/>
     </row>
     <row r="684">
-      <c r="D684" s="8"/>
+      <c r="D684" s="9"/>
     </row>
     <row r="685">
-      <c r="D685" s="8"/>
+      <c r="D685" s="9"/>
     </row>
     <row r="686">
-      <c r="D686" s="8"/>
+      <c r="D686" s="9"/>
     </row>
     <row r="687">
-      <c r="D687" s="8"/>
+      <c r="D687" s="9"/>
     </row>
     <row r="688">
-      <c r="D688" s="8"/>
+      <c r="D688" s="9"/>
     </row>
     <row r="689">
-      <c r="D689" s="8"/>
+      <c r="D689" s="9"/>
     </row>
     <row r="690">
-      <c r="D690" s="8"/>
+      <c r="D690" s="9"/>
     </row>
     <row r="691">
-      <c r="D691" s="8"/>
+      <c r="D691" s="9"/>
     </row>
     <row r="692">
-      <c r="D692" s="8"/>
+      <c r="D692" s="9"/>
     </row>
     <row r="693">
-      <c r="D693" s="8"/>
+      <c r="D693" s="9"/>
     </row>
     <row r="694">
-      <c r="D694" s="8"/>
+      <c r="D694" s="9"/>
     </row>
     <row r="695">
-      <c r="D695" s="8"/>
+      <c r="D695" s="9"/>
     </row>
     <row r="696">
-      <c r="D696" s="8"/>
+      <c r="D696" s="9"/>
     </row>
     <row r="697">
-      <c r="D697" s="8"/>
+      <c r="D697" s="9"/>
     </row>
     <row r="698">
-      <c r="D698" s="8"/>
+      <c r="D698" s="9"/>
     </row>
     <row r="699">
-      <c r="D699" s="8"/>
+      <c r="D699" s="9"/>
     </row>
     <row r="700">
-      <c r="D700" s="8"/>
+      <c r="D700" s="9"/>
     </row>
     <row r="701">
-      <c r="D701" s="8"/>
+      <c r="D701" s="9"/>
     </row>
     <row r="702">
-      <c r="D702" s="8"/>
+      <c r="D702" s="9"/>
     </row>
     <row r="703">
-      <c r="D703" s="8"/>
+      <c r="D703" s="9"/>
     </row>
     <row r="704">
-      <c r="D704" s="8"/>
+      <c r="D704" s="9"/>
     </row>
     <row r="705">
-      <c r="D705" s="8"/>
+      <c r="D705" s="9"/>
     </row>
     <row r="706">
-      <c r="D706" s="8"/>
+      <c r="D706" s="9"/>
     </row>
     <row r="707">
-      <c r="D707" s="8"/>
+      <c r="D707" s="9"/>
     </row>
     <row r="708">
-      <c r="D708" s="8"/>
+      <c r="D708" s="9"/>
     </row>
     <row r="709">
-      <c r="D709" s="8"/>
+      <c r="D709" s="9"/>
     </row>
     <row r="710">
-      <c r="D710" s="8"/>
+      <c r="D710" s="9"/>
     </row>
     <row r="711">
-      <c r="D711" s="8"/>
+      <c r="D711" s="9"/>
     </row>
     <row r="712">
-      <c r="D712" s="8"/>
+      <c r="D712" s="9"/>
     </row>
     <row r="713">
-      <c r="D713" s="8"/>
+      <c r="D713" s="9"/>
     </row>
     <row r="714">
-      <c r="D714" s="8"/>
+      <c r="D714" s="9"/>
     </row>
     <row r="715">
-      <c r="D715" s="8"/>
+      <c r="D715" s="9"/>
     </row>
     <row r="716">
-      <c r="D716" s="8"/>
+      <c r="D716" s="9"/>
     </row>
     <row r="717">
-      <c r="D717" s="8"/>
+      <c r="D717" s="9"/>
     </row>
     <row r="718">
-      <c r="D718" s="8"/>
+      <c r="D718" s="9"/>
     </row>
     <row r="719">
-      <c r="D719" s="8"/>
+      <c r="D719" s="9"/>
     </row>
     <row r="720">
-      <c r="D720" s="8"/>
+      <c r="D720" s="9"/>
     </row>
     <row r="721">
-      <c r="D721" s="8"/>
+      <c r="D721" s="9"/>
     </row>
     <row r="722">
-      <c r="D722" s="8"/>
+      <c r="D722" s="9"/>
     </row>
     <row r="723">
-      <c r="D723" s="8"/>
+      <c r="D723" s="9"/>
     </row>
     <row r="724">
-      <c r="D724" s="8"/>
+      <c r="D724" s="9"/>
     </row>
     <row r="725">
-      <c r="D725" s="8"/>
+      <c r="D725" s="9"/>
     </row>
     <row r="726">
-      <c r="D726" s="8"/>
+      <c r="D726" s="9"/>
     </row>
     <row r="727">
-      <c r="D727" s="8"/>
+      <c r="D727" s="9"/>
     </row>
     <row r="728">
-      <c r="D728" s="8"/>
+      <c r="D728" s="9"/>
     </row>
     <row r="729">
-      <c r="D729" s="8"/>
+      <c r="D729" s="9"/>
     </row>
     <row r="730">
-      <c r="D730" s="8"/>
+      <c r="D730" s="9"/>
     </row>
     <row r="731">
-      <c r="D731" s="8"/>
+      <c r="D731" s="9"/>
     </row>
     <row r="732">
-      <c r="D732" s="8"/>
+      <c r="D732" s="9"/>
     </row>
     <row r="733">
-      <c r="D733" s="8"/>
+      <c r="D733" s="9"/>
     </row>
     <row r="734">
-      <c r="D734" s="8"/>
+      <c r="D734" s="9"/>
     </row>
     <row r="735">
-      <c r="D735" s="8"/>
+      <c r="D735" s="9"/>
     </row>
     <row r="736">
-      <c r="D736" s="8"/>
+      <c r="D736" s="9"/>
     </row>
     <row r="737">
-      <c r="D737" s="8"/>
+      <c r="D737" s="9"/>
     </row>
     <row r="738">
-      <c r="D738" s="8"/>
+      <c r="D738" s="9"/>
     </row>
     <row r="739">
-      <c r="D739" s="8"/>
+      <c r="D739" s="9"/>
     </row>
     <row r="740">
-      <c r="D740" s="8"/>
+      <c r="D740" s="9"/>
     </row>
     <row r="741">
-      <c r="D741" s="8"/>
+      <c r="D741" s="9"/>
     </row>
     <row r="742">
-      <c r="D742" s="8"/>
+      <c r="D742" s="9"/>
     </row>
     <row r="743">
-      <c r="D743" s="8"/>
+      <c r="D743" s="9"/>
     </row>
     <row r="744">
-      <c r="D744" s="8"/>
+      <c r="D744" s="9"/>
     </row>
     <row r="745">
-      <c r="D745" s="8"/>
+      <c r="D745" s="9"/>
     </row>
     <row r="746">
-      <c r="D746" s="8"/>
+      <c r="D746" s="9"/>
     </row>
     <row r="747">
-      <c r="D747" s="8"/>
+      <c r="D747" s="9"/>
     </row>
     <row r="748">
-      <c r="D748" s="8"/>
+      <c r="D748" s="9"/>
     </row>
     <row r="749">
-      <c r="D749" s="8"/>
+      <c r="D749" s="9"/>
     </row>
     <row r="750">
-      <c r="D750" s="8"/>
+      <c r="D750" s="9"/>
     </row>
     <row r="751">
-      <c r="D751" s="8"/>
+      <c r="D751" s="9"/>
     </row>
     <row r="752">
-      <c r="D752" s="8"/>
+      <c r="D752" s="9"/>
     </row>
     <row r="753">
-      <c r="D753" s="8"/>
+      <c r="D753" s="9"/>
     </row>
     <row r="754">
-      <c r="D754" s="8"/>
+      <c r="D754" s="9"/>
     </row>
     <row r="755">
-      <c r="D755" s="8"/>
+      <c r="D755" s="9"/>
     </row>
     <row r="756">
-      <c r="D756" s="8"/>
+      <c r="D756" s="9"/>
     </row>
     <row r="757">
-      <c r="D757" s="8"/>
+      <c r="D757" s="9"/>
     </row>
     <row r="758">
-      <c r="D758" s="8"/>
+      <c r="D758" s="9"/>
     </row>
     <row r="759">
-      <c r="D759" s="8"/>
+      <c r="D759" s="9"/>
     </row>
     <row r="760">
-      <c r="D760" s="8"/>
+      <c r="D760" s="9"/>
     </row>
     <row r="761">
-      <c r="D761" s="8"/>
+      <c r="D761" s="9"/>
     </row>
     <row r="762">
-      <c r="D762" s="8"/>
+      <c r="D762" s="9"/>
     </row>
     <row r="763">
-      <c r="D763" s="8"/>
+      <c r="D763" s="9"/>
     </row>
     <row r="764">
-      <c r="D764" s="8"/>
+      <c r="D764" s="9"/>
     </row>
     <row r="765">
-      <c r="D765" s="8"/>
+      <c r="D765" s="9"/>
     </row>
     <row r="766">
-      <c r="D766" s="8"/>
+      <c r="D766" s="9"/>
     </row>
     <row r="767">
-      <c r="D767" s="8"/>
+      <c r="D767" s="9"/>
     </row>
     <row r="768">
-      <c r="D768" s="8"/>
+      <c r="D768" s="9"/>
     </row>
     <row r="769">
-      <c r="D769" s="8"/>
+      <c r="D769" s="9"/>
     </row>
     <row r="770">
-      <c r="D770" s="8"/>
+      <c r="D770" s="9"/>
     </row>
     <row r="771">
-      <c r="D771" s="8"/>
+      <c r="D771" s="9"/>
     </row>
     <row r="772">
-      <c r="D772" s="8"/>
+      <c r="D772" s="9"/>
     </row>
     <row r="773">
-      <c r="D773" s="8"/>
+      <c r="D773" s="9"/>
     </row>
     <row r="774">
-      <c r="D774" s="8"/>
+      <c r="D774" s="9"/>
     </row>
     <row r="775">
-      <c r="D775" s="8"/>
+      <c r="D775" s="9"/>
     </row>
     <row r="776">
-      <c r="D776" s="8"/>
+      <c r="D776" s="9"/>
     </row>
     <row r="777">
-      <c r="D777" s="8"/>
+      <c r="D777" s="9"/>
     </row>
     <row r="778">
-      <c r="D778" s="8"/>
+      <c r="D778" s="9"/>
     </row>
     <row r="779">
-      <c r="D779" s="8"/>
+      <c r="D779" s="9"/>
     </row>
     <row r="780">
-      <c r="D780" s="8"/>
+      <c r="D780" s="9"/>
     </row>
     <row r="781">
-      <c r="D781" s="8"/>
+      <c r="D781" s="9"/>
     </row>
     <row r="782">
-      <c r="D782" s="8"/>
+      <c r="D782" s="9"/>
     </row>
     <row r="783">
-      <c r="D783" s="8"/>
+      <c r="D783" s="9"/>
     </row>
     <row r="784">
-      <c r="D784" s="8"/>
+      <c r="D784" s="9"/>
     </row>
     <row r="785">
-      <c r="D785" s="8"/>
+      <c r="D785" s="9"/>
     </row>
     <row r="786">
-      <c r="D786" s="8"/>
+      <c r="D786" s="9"/>
     </row>
     <row r="787">
-      <c r="D787" s="8"/>
+      <c r="D787" s="9"/>
     </row>
     <row r="788">
-      <c r="D788" s="8"/>
+      <c r="D788" s="9"/>
     </row>
     <row r="789">
-      <c r="D789" s="8"/>
+      <c r="D789" s="9"/>
     </row>
     <row r="790">
-      <c r="D790" s="8"/>
+      <c r="D790" s="9"/>
     </row>
     <row r="791">
-      <c r="D791" s="8"/>
+      <c r="D791" s="9"/>
     </row>
     <row r="792">
-      <c r="D792" s="8"/>
+      <c r="D792" s="9"/>
     </row>
     <row r="793">
-      <c r="D793" s="8"/>
+      <c r="D793" s="9"/>
     </row>
     <row r="794">
-      <c r="D794" s="8"/>
+      <c r="D794" s="9"/>
     </row>
     <row r="795">
-      <c r="D795" s="8"/>
+      <c r="D795" s="9"/>
     </row>
     <row r="796">
-      <c r="D796" s="8"/>
+      <c r="D796" s="9"/>
     </row>
     <row r="797">
-      <c r="D797" s="8"/>
+      <c r="D797" s="9"/>
     </row>
     <row r="798">
-      <c r="D798" s="8"/>
+      <c r="D798" s="9"/>
     </row>
     <row r="799">
-      <c r="D799" s="8"/>
+      <c r="D799" s="9"/>
     </row>
     <row r="800">
-      <c r="D800" s="8"/>
+      <c r="D800" s="9"/>
     </row>
     <row r="801">
-      <c r="D801" s="8"/>
+      <c r="D801" s="9"/>
     </row>
     <row r="802">
-      <c r="D802" s="8"/>
+      <c r="D802" s="9"/>
     </row>
     <row r="803">
-      <c r="D803" s="8"/>
+      <c r="D803" s="9"/>
     </row>
     <row r="804">
-      <c r="D804" s="8"/>
+      <c r="D804" s="9"/>
     </row>
     <row r="805">
-      <c r="D805" s="8"/>
+      <c r="D805" s="9"/>
     </row>
     <row r="806">
-      <c r="D806" s="8"/>
+      <c r="D806" s="9"/>
     </row>
     <row r="807">
-      <c r="D807" s="8"/>
+      <c r="D807" s="9"/>
     </row>
     <row r="808">
-      <c r="D808" s="8"/>
+      <c r="D808" s="9"/>
     </row>
     <row r="809">
-      <c r="D809" s="8"/>
+      <c r="D809" s="9"/>
     </row>
     <row r="810">
-      <c r="D810" s="8"/>
+      <c r="D810" s="9"/>
     </row>
     <row r="811">
-      <c r="D811" s="8"/>
+      <c r="D811" s="9"/>
     </row>
     <row r="812">
-      <c r="D812" s="8"/>
+      <c r="D812" s="9"/>
     </row>
     <row r="813">
-      <c r="D813" s="8"/>
+      <c r="D813" s="9"/>
     </row>
     <row r="814">
-      <c r="D814" s="8"/>
+      <c r="D814" s="9"/>
     </row>
     <row r="815">
-      <c r="D815" s="8"/>
+      <c r="D815" s="9"/>
     </row>
     <row r="816">
-      <c r="D816" s="8"/>
+      <c r="D816" s="9"/>
     </row>
     <row r="817">
-      <c r="D817" s="8"/>
+      <c r="D817" s="9"/>
     </row>
     <row r="818">
-      <c r="D818" s="8"/>
+      <c r="D818" s="9"/>
     </row>
     <row r="819">
-      <c r="D819" s="8"/>
+      <c r="D819" s="9"/>
     </row>
     <row r="820">
-      <c r="D820" s="8"/>
+      <c r="D820" s="9"/>
     </row>
     <row r="821">
-      <c r="D821" s="8"/>
+      <c r="D821" s="9"/>
     </row>
     <row r="822">
-      <c r="D822" s="8"/>
+      <c r="D822" s="9"/>
     </row>
     <row r="823">
-      <c r="D823" s="8"/>
+      <c r="D823" s="9"/>
     </row>
     <row r="824">
-      <c r="D824" s="8"/>
+      <c r="D824" s="9"/>
     </row>
     <row r="825">
-      <c r="D825" s="8"/>
+      <c r="D825" s="9"/>
     </row>
     <row r="826">
-      <c r="D826" s="8"/>
+      <c r="D826" s="9"/>
     </row>
     <row r="827">
-      <c r="D827" s="8"/>
+      <c r="D827" s="9"/>
     </row>
     <row r="828">
-      <c r="D828" s="8"/>
+      <c r="D828" s="9"/>
     </row>
     <row r="829">
-      <c r="D829" s="8"/>
+      <c r="D829" s="9"/>
     </row>
     <row r="830">
-      <c r="D830" s="8"/>
+      <c r="D830" s="9"/>
     </row>
     <row r="831">
-      <c r="D831" s="8"/>
+      <c r="D831" s="9"/>
     </row>
     <row r="832">
-      <c r="D832" s="8"/>
+      <c r="D832" s="9"/>
     </row>
     <row r="833">
-      <c r="D833" s="8"/>
+      <c r="D833" s="9"/>
     </row>
     <row r="834">
-      <c r="D834" s="8"/>
+      <c r="D834" s="9"/>
     </row>
     <row r="835">
-      <c r="D835" s="8"/>
+      <c r="D835" s="9"/>
     </row>
     <row r="836">
-      <c r="D836" s="8"/>
+      <c r="D836" s="9"/>
     </row>
     <row r="837">
-      <c r="D837" s="8"/>
+      <c r="D837" s="9"/>
     </row>
     <row r="838">
-      <c r="D838" s="8"/>
+      <c r="D838" s="9"/>
     </row>
     <row r="839">
-      <c r="D839" s="8"/>
+      <c r="D839" s="9"/>
     </row>
     <row r="840">
-      <c r="D840" s="8"/>
+      <c r="D840" s="9"/>
     </row>
     <row r="841">
-      <c r="D841" s="8"/>
+      <c r="D841" s="9"/>
     </row>
     <row r="842">
-      <c r="D842" s="8"/>
+      <c r="D842" s="9"/>
     </row>
     <row r="843">
-      <c r="D843" s="8"/>
+      <c r="D843" s="9"/>
     </row>
     <row r="844">
-      <c r="D844" s="8"/>
+      <c r="D844" s="9"/>
     </row>
     <row r="845">
-      <c r="D845" s="8"/>
+      <c r="D845" s="9"/>
     </row>
     <row r="846">
-      <c r="D846" s="8"/>
+      <c r="D846" s="9"/>
     </row>
     <row r="847">
-      <c r="D847" s="8"/>
+      <c r="D847" s="9"/>
     </row>
     <row r="848">
-      <c r="D848" s="8"/>
+      <c r="D848" s="9"/>
     </row>
     <row r="849">
-      <c r="D849" s="8"/>
+      <c r="D849" s="9"/>
     </row>
     <row r="850">
-      <c r="D850" s="8"/>
+      <c r="D850" s="9"/>
     </row>
     <row r="851">
-      <c r="D851" s="8"/>
+      <c r="D851" s="9"/>
     </row>
     <row r="852">
-      <c r="D852" s="8"/>
+      <c r="D852" s="9"/>
     </row>
     <row r="853">
-      <c r="D853" s="8"/>
+      <c r="D853" s="9"/>
     </row>
     <row r="854">
-      <c r="D854" s="8"/>
+      <c r="D854" s="9"/>
     </row>
     <row r="855">
-      <c r="D855" s="8"/>
+      <c r="D855" s="9"/>
     </row>
     <row r="856">
-      <c r="D856" s="8"/>
+      <c r="D856" s="9"/>
     </row>
     <row r="857">
-      <c r="D857" s="8"/>
+      <c r="D857" s="9"/>
     </row>
     <row r="858">
-      <c r="D858" s="8"/>
+      <c r="D858" s="9"/>
     </row>
     <row r="859">
-      <c r="D859" s="8"/>
+      <c r="D859" s="9"/>
     </row>
     <row r="860">
-      <c r="D860" s="8"/>
+      <c r="D860" s="9"/>
     </row>
     <row r="861">
-      <c r="D861" s="8"/>
+      <c r="D861" s="9"/>
     </row>
     <row r="862">
-      <c r="D862" s="8"/>
+      <c r="D862" s="9"/>
     </row>
     <row r="863">
-      <c r="D863" s="8"/>
+      <c r="D863" s="9"/>
     </row>
     <row r="864">
-      <c r="D864" s="8"/>
+      <c r="D864" s="9"/>
     </row>
     <row r="865">
-      <c r="D865" s="8"/>
+      <c r="D865" s="9"/>
     </row>
     <row r="866">
-      <c r="D866" s="8"/>
+      <c r="D866" s="9"/>
     </row>
     <row r="867">
-      <c r="D867" s="8"/>
+      <c r="D867" s="9"/>
     </row>
     <row r="868">
-      <c r="D868" s="8"/>
+      <c r="D868" s="9"/>
     </row>
     <row r="869">
-      <c r="D869" s="8"/>
+      <c r="D869" s="9"/>
     </row>
     <row r="870">
-      <c r="D870" s="8"/>
+      <c r="D870" s="9"/>
     </row>
     <row r="871">
-      <c r="D871" s="8"/>
+      <c r="D871" s="9"/>
     </row>
     <row r="872">
-      <c r="D872" s="8"/>
+      <c r="D872" s="9"/>
     </row>
     <row r="873">
-      <c r="D873" s="8"/>
+      <c r="D873" s="9"/>
     </row>
     <row r="874">
-      <c r="D874" s="8"/>
+      <c r="D874" s="9"/>
     </row>
     <row r="875">
-      <c r="D875" s="8"/>
+      <c r="D875" s="9"/>
     </row>
     <row r="876">
-      <c r="D876" s="8"/>
+      <c r="D876" s="9"/>
     </row>
     <row r="877">
-      <c r="D877" s="8"/>
+      <c r="D877" s="9"/>
     </row>
     <row r="878">
-      <c r="D878" s="8"/>
+      <c r="D878" s="9"/>
     </row>
     <row r="879">
-      <c r="D879" s="8"/>
+      <c r="D879" s="9"/>
     </row>
     <row r="880">
-      <c r="D880" s="8"/>
+      <c r="D880" s="9"/>
     </row>
     <row r="881">
-      <c r="D881" s="8"/>
+      <c r="D881" s="9"/>
     </row>
     <row r="882">
-      <c r="D882" s="8"/>
+      <c r="D882" s="9"/>
     </row>
     <row r="883">
-      <c r="D883" s="8"/>
+      <c r="D883" s="9"/>
     </row>
     <row r="884">
-      <c r="D884" s="8"/>
+      <c r="D884" s="9"/>
     </row>
     <row r="885">
-      <c r="D885" s="8"/>
+      <c r="D885" s="9"/>
     </row>
     <row r="886">
-      <c r="D886" s="8"/>
+      <c r="D886" s="9"/>
     </row>
     <row r="887">
-      <c r="D887" s="8"/>
+      <c r="D887" s="9"/>
     </row>
     <row r="888">
-      <c r="D888" s="8"/>
+      <c r="D888" s="9"/>
     </row>
     <row r="889">
-      <c r="D889" s="8"/>
+      <c r="D889" s="9"/>
     </row>
     <row r="890">
-      <c r="D890" s="8"/>
+      <c r="D890" s="9"/>
     </row>
     <row r="891">
-      <c r="D891" s="8"/>
+      <c r="D891" s="9"/>
     </row>
     <row r="892">
-      <c r="D892" s="8"/>
+      <c r="D892" s="9"/>
     </row>
     <row r="893">
-      <c r="D893" s="8"/>
+      <c r="D893" s="9"/>
     </row>
     <row r="894">
-      <c r="D894" s="8"/>
+      <c r="D894" s="9"/>
     </row>
     <row r="895">
-      <c r="D895" s="8"/>
+      <c r="D895" s="9"/>
     </row>
     <row r="896">
-      <c r="D896" s="8"/>
+      <c r="D896" s="9"/>
     </row>
     <row r="897">
-      <c r="D897" s="8"/>
+      <c r="D897" s="9"/>
     </row>
     <row r="898">
-      <c r="D898" s="8"/>
+      <c r="D898" s="9"/>
     </row>
     <row r="899">
-      <c r="D899" s="8"/>
+      <c r="D899" s="9"/>
     </row>
     <row r="900">
-      <c r="D900" s="8"/>
+      <c r="D900" s="9"/>
     </row>
     <row r="901">
-      <c r="D901" s="8"/>
+      <c r="D901" s="9"/>
     </row>
     <row r="902">
-      <c r="D902" s="8"/>
+      <c r="D902" s="9"/>
     </row>
     <row r="903">
-      <c r="D903" s="8"/>
+      <c r="D903" s="9"/>
     </row>
     <row r="904">
-      <c r="D904" s="8"/>
+      <c r="D904" s="9"/>
     </row>
     <row r="905">
-      <c r="D905" s="8"/>
+      <c r="D905" s="9"/>
     </row>
     <row r="906">
-      <c r="D906" s="8"/>
+      <c r="D906" s="9"/>
     </row>
     <row r="907">
-      <c r="D907" s="8"/>
+      <c r="D907" s="9"/>
     </row>
     <row r="908">
-      <c r="D908" s="8"/>
+      <c r="D908" s="9"/>
     </row>
     <row r="909">
-      <c r="D909" s="8"/>
+      <c r="D909" s="9"/>
     </row>
     <row r="910">
-      <c r="D910" s="8"/>
+      <c r="D910" s="9"/>
     </row>
     <row r="911">
-      <c r="D911" s="8"/>
+      <c r="D911" s="9"/>
     </row>
     <row r="912">
-      <c r="D912" s="8"/>
+      <c r="D912" s="9"/>
     </row>
     <row r="913">
-      <c r="D913" s="8"/>
+      <c r="D913" s="9"/>
     </row>
     <row r="914">
-      <c r="D914" s="8"/>
+      <c r="D914" s="9"/>
     </row>
     <row r="915">
-      <c r="D915" s="8"/>
+      <c r="D915" s="9"/>
     </row>
     <row r="916">
-      <c r="D916" s="8"/>
+      <c r="D916" s="9"/>
     </row>
     <row r="917">
-      <c r="D917" s="8"/>
+      <c r="D917" s="9"/>
     </row>
     <row r="918">
-      <c r="D918" s="8"/>
+      <c r="D918" s="9"/>
     </row>
     <row r="919">
-      <c r="D919" s="8"/>
+      <c r="D919" s="9"/>
     </row>
     <row r="920">
-      <c r="D920" s="8"/>
+      <c r="D920" s="9"/>
     </row>
     <row r="921">
-      <c r="D921" s="8"/>
+      <c r="D921" s="9"/>
     </row>
     <row r="922">
-      <c r="D922" s="8"/>
+      <c r="D922" s="9"/>
     </row>
     <row r="923">
-      <c r="D923" s="8"/>
+      <c r="D923" s="9"/>
     </row>
     <row r="924">
-      <c r="D924" s="8"/>
+      <c r="D924" s="9"/>
     </row>
     <row r="925">
-      <c r="D925" s="8"/>
+      <c r="D925" s="9"/>
     </row>
     <row r="926">
-      <c r="D926" s="8"/>
+      <c r="D926" s="9"/>
     </row>
     <row r="927">
-      <c r="D927" s="8"/>
+      <c r="D927" s="9"/>
     </row>
     <row r="928">
-      <c r="D928" s="8"/>
+      <c r="D928" s="9"/>
     </row>
     <row r="929">
-      <c r="D929" s="8"/>
+      <c r="D929" s="9"/>
     </row>
     <row r="930">
-      <c r="D930" s="8"/>
+      <c r="D930" s="9"/>
     </row>
     <row r="931">
-      <c r="D931" s="8"/>
+      <c r="D931" s="9"/>
     </row>
     <row r="932">
-      <c r="D932" s="8"/>
+      <c r="D932" s="9"/>
     </row>
     <row r="933">
-      <c r="D933" s="8"/>
+      <c r="D933" s="9"/>
     </row>
     <row r="934">
-      <c r="D934" s="8"/>
+      <c r="D934" s="9"/>
     </row>
     <row r="935">
-      <c r="D935" s="8"/>
+      <c r="D935" s="9"/>
     </row>
     <row r="936">
-      <c r="D936" s="8"/>
+      <c r="D936" s="9"/>
     </row>
     <row r="937">
-      <c r="D937" s="8"/>
+      <c r="D937" s="9"/>
     </row>
     <row r="938">
-      <c r="D938" s="8"/>
+      <c r="D938" s="9"/>
     </row>
     <row r="939">
-      <c r="D939" s="8"/>
+      <c r="D939" s="9"/>
     </row>
     <row r="940">
-      <c r="D940" s="8"/>
+      <c r="D940" s="9"/>
     </row>
     <row r="941">
-      <c r="D941" s="8"/>
+      <c r="D941" s="9"/>
     </row>
     <row r="942">
-      <c r="D942" s="8"/>
+      <c r="D942" s="9"/>
     </row>
     <row r="943">
-      <c r="D943" s="8"/>
+      <c r="D943" s="9"/>
     </row>
     <row r="944">
-      <c r="D944" s="8"/>
+      <c r="D944" s="9"/>
     </row>
     <row r="945">
-      <c r="D945" s="8"/>
+      <c r="D945" s="9"/>
     </row>
     <row r="946">
-      <c r="D946" s="8"/>
+      <c r="D946" s="9"/>
     </row>
     <row r="947">
-      <c r="D947" s="8"/>
+      <c r="D947" s="9"/>
     </row>
     <row r="948">
-      <c r="D948" s="8"/>
+      <c r="D948" s="9"/>
     </row>
     <row r="949">
-      <c r="D949" s="8"/>
+      <c r="D949" s="9"/>
     </row>
     <row r="950">
-      <c r="D950" s="8"/>
+      <c r="D950" s="9"/>
     </row>
     <row r="951">
-      <c r="D951" s="8"/>
+      <c r="D951" s="9"/>
     </row>
     <row r="952">
-      <c r="D952" s="8"/>
+      <c r="D952" s="9"/>
     </row>
     <row r="953">
-      <c r="D953" s="8"/>
+      <c r="D953" s="9"/>
     </row>
     <row r="954">
-      <c r="D954" s="8"/>
+      <c r="D954" s="9"/>
     </row>
     <row r="955">
-      <c r="D955" s="8"/>
+      <c r="D955" s="9"/>
     </row>
     <row r="956">
-      <c r="D956" s="8"/>
+      <c r="D956" s="9"/>
     </row>
     <row r="957">
-      <c r="D957" s="8"/>
+      <c r="D957" s="9"/>
     </row>
     <row r="958">
-      <c r="D958" s="8"/>
+      <c r="D958" s="9"/>
     </row>
     <row r="959">
-      <c r="D959" s="8"/>
+      <c r="D959" s="9"/>
     </row>
     <row r="960">
-      <c r="D960" s="8"/>
+      <c r="D960" s="9"/>
     </row>
     <row r="961">
-      <c r="D961" s="8"/>
+      <c r="D961" s="9"/>
     </row>
     <row r="962">
-      <c r="D962" s="8"/>
+      <c r="D962" s="9"/>
     </row>
     <row r="963">
-      <c r="D963" s="8"/>
+      <c r="D963" s="9"/>
     </row>
     <row r="964">
-      <c r="D964" s="8"/>
+      <c r="D964" s="9"/>
     </row>
     <row r="965">
-      <c r="D965" s="8"/>
+      <c r="D965" s="9"/>
     </row>
     <row r="966">
-      <c r="D966" s="8"/>
+      <c r="D966" s="9"/>
     </row>
     <row r="967">
-      <c r="D967" s="8"/>
+      <c r="D967" s="9"/>
     </row>
     <row r="968">
-      <c r="D968" s="8"/>
+      <c r="D968" s="9"/>
     </row>
     <row r="969">
-      <c r="D969" s="8"/>
+      <c r="D969" s="9"/>
     </row>
     <row r="970">
-      <c r="D970" s="8"/>
+      <c r="D970" s="9"/>
     </row>
     <row r="971">
-      <c r="D971" s="8"/>
+      <c r="D971" s="9"/>
     </row>
     <row r="972">
-      <c r="D972" s="8"/>
+      <c r="D972" s="9"/>
     </row>
     <row r="973">
-      <c r="D973" s="8"/>
+      <c r="D973" s="9"/>
     </row>
     <row r="974">
-      <c r="D974" s="8"/>
+      <c r="D974" s="9"/>
     </row>
     <row r="975">
-      <c r="D975" s="8"/>
+      <c r="D975" s="9"/>
     </row>
     <row r="976">
-      <c r="D976" s="8"/>
+      <c r="D976" s="9"/>
     </row>
     <row r="977">
-      <c r="D977" s="8"/>
+      <c r="D977" s="9"/>
     </row>
     <row r="978">
-      <c r="D978" s="8"/>
+      <c r="D978" s="9"/>
     </row>
     <row r="979">
-      <c r="D979" s="8"/>
+      <c r="D979" s="9"/>
     </row>
     <row r="980">
-      <c r="D980" s="8"/>
+      <c r="D980" s="9"/>
     </row>
     <row r="981">
-      <c r="D981" s="8"/>
+      <c r="D981" s="9"/>
     </row>
     <row r="982">
-      <c r="D982" s="8"/>
+      <c r="D982" s="9"/>
     </row>
     <row r="983">
-      <c r="D983" s="8"/>
+      <c r="D983" s="9"/>
     </row>
     <row r="984">
-      <c r="D984" s="8"/>
+      <c r="D984" s="9"/>
     </row>
     <row r="985">
-      <c r="D985" s="8"/>
+      <c r="D985" s="9"/>
     </row>
     <row r="986">
-      <c r="D986" s="8"/>
+      <c r="D986" s="9"/>
     </row>
     <row r="987">
-      <c r="D987" s="8"/>
+      <c r="D987" s="9"/>
     </row>
     <row r="988">
-      <c r="D988" s="8"/>
+      <c r="D988" s="9"/>
     </row>
     <row r="989">
-      <c r="D989" s="8"/>
+      <c r="D989" s="9"/>
     </row>
     <row r="990">
-      <c r="D990" s="8"/>
+      <c r="D990" s="9"/>
     </row>
     <row r="991">
-      <c r="D991" s="8"/>
+      <c r="D991" s="9"/>
     </row>
     <row r="992">
-      <c r="D992" s="8"/>
+      <c r="D992" s="9"/>
     </row>
     <row r="993">
-      <c r="D993" s="8"/>
+      <c r="D993" s="9"/>
     </row>
     <row r="994">
-      <c r="D994" s="8"/>
+      <c r="D994" s="9"/>
     </row>
     <row r="995">
-      <c r="D995" s="8"/>
+      <c r="D995" s="9"/>
     </row>
     <row r="996">
-      <c r="D996" s="8"/>
+      <c r="D996" s="9"/>
     </row>
     <row r="997">
-      <c r="D997" s="8"/>
+      <c r="D997" s="9"/>
     </row>
     <row r="998">
-      <c r="D998" s="8"/>
+      <c r="D998" s="9"/>
     </row>
     <row r="999">
-      <c r="D999" s="8"/>
+      <c r="D999" s="9"/>
     </row>
     <row r="1000">
-      <c r="D1000" s="8"/>
+      <c r="D1000" s="9"/>
     </row>
   </sheetData>
   <printOptions gridLines="1" horizontalCentered="1"/>
@@ -4241,7 +4400,7 @@
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <headerFooter>
     <oddHeader>&amp;LChelmsford Summer Beer &amp;&amp; Cider Festival 2018&amp;RBrewery Bar Listings</oddHeader>
-    <oddFooter>&amp;LLast updated 30/06/2018&amp;Rwww.cbcf.info/brewery-bars</oddFooter>
+    <oddFooter>&amp;LLast updated 03/07/2018&amp;Rwww.cbcf.info/brewery-bars</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>